<commit_message>
perfil de admin y teacher listos, trabajando en student
</commit_message>
<xml_diff>
--- a/excel/estudiantes.xlsx
+++ b/excel/estudiantes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CASA\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFDC0F46-9083-4362-BC21-3EDEF9C38FA8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D8C67C9-CAB1-4C49-B9FB-00185DA3D250}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{62705D06-57FD-4738-A289-6DD2C028AABD}"/>
   </bookViews>
@@ -50,9 +50,6 @@
     <t>EMAIL</t>
   </si>
   <si>
-    <t>INSTITUCION</t>
-  </si>
-  <si>
     <t>ASTRONOMYAPP</t>
   </si>
   <si>
@@ -61,12 +58,15 @@
   <si>
     <t>RUT</t>
   </si>
+  <si>
+    <t>DV</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -113,6 +113,14 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -310,11 +318,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -328,9 +337,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -372,8 +378,12 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
+    <cellStyle name="Hipervínculo" xfId="4" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{24B2CEEC-DDD5-49FA-BADB-F6E46AAC1E32}"/>
     <cellStyle name="Normal 3" xfId="2" xr:uid="{3B182533-9141-472D-909A-6287539AB109}"/>
@@ -692,31 +702,31 @@
   <dimension ref="B1:O199"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.42578125" customWidth="1"/>
-    <col min="2" max="2" width="20" customWidth="1"/>
-    <col min="3" max="3" width="25.5703125" customWidth="1"/>
-    <col min="4" max="4" width="26" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" customWidth="1"/>
+    <col min="2" max="2" width="27.42578125" customWidth="1"/>
+    <col min="3" max="3" width="28.42578125" customWidth="1"/>
+    <col min="4" max="4" width="30.140625" customWidth="1"/>
     <col min="5" max="5" width="19.5703125" customWidth="1"/>
-    <col min="6" max="6" width="38.5703125" customWidth="1"/>
-    <col min="7" max="7" width="34.42578125" customWidth="1"/>
+    <col min="6" max="6" width="6.140625" customWidth="1"/>
+    <col min="7" max="7" width="40.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:15" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="15" t="s">
-        <v>6</v>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="14" t="s">
+        <v>5</v>
       </c>
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
@@ -728,14 +738,14 @@
       <c r="O2" s="5"/>
     </row>
     <row r="3" spans="2:15" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="16" t="s">
-        <v>7</v>
+      <c r="B3" s="15" t="s">
+        <v>6</v>
       </c>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="8"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="7"/>
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
@@ -756,13 +766,13 @@
         <v>2</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>5</v>
       </c>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
@@ -774,12 +784,12 @@
       <c r="O4" s="2"/>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B5" s="9"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="11"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="20"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
@@ -790,12 +800,12 @@
       <c r="O5" s="3"/>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B6" s="9"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="11"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="20"/>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
@@ -806,12 +816,12 @@
       <c r="O6" s="3"/>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B7" s="9"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="11"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="10"/>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
@@ -822,12 +832,12 @@
       <c r="O7" s="3"/>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B8" s="9"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="11"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="10"/>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
@@ -838,12 +848,12 @@
       <c r="O8" s="3"/>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B9" s="9"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="11"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="10"/>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
@@ -854,12 +864,12 @@
       <c r="O9" s="3"/>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B10" s="9"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="11"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="10"/>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
@@ -870,12 +880,12 @@
       <c r="O10" s="3"/>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B11" s="9"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="11"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="10"/>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
@@ -886,12 +896,12 @@
       <c r="O11" s="3"/>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B12" s="9"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="11"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="10"/>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
@@ -902,12 +912,12 @@
       <c r="O12" s="3"/>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B13" s="9"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="11"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="10"/>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
@@ -918,12 +928,12 @@
       <c r="O13" s="3"/>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B14" s="9"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="11"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="10"/>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
@@ -934,12 +944,12 @@
       <c r="O14" s="3"/>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B15" s="9"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="11"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="10"/>
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
@@ -950,12 +960,12 @@
       <c r="O15" s="3"/>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B16" s="9"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="11"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="10"/>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
@@ -966,12 +976,12 @@
       <c r="O16" s="3"/>
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B17" s="9"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="11"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="10"/>
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
@@ -982,12 +992,12 @@
       <c r="O17" s="3"/>
     </row>
     <row r="18" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B18" s="9"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="11"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="10"/>
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
@@ -998,12 +1008,12 @@
       <c r="O18" s="3"/>
     </row>
     <row r="19" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B19" s="9"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="11"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="10"/>
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
@@ -1014,12 +1024,12 @@
       <c r="O19" s="3"/>
     </row>
     <row r="20" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B20" s="9"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="10"/>
-      <c r="G20" s="11"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="10"/>
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
@@ -1030,12 +1040,12 @@
       <c r="O20" s="3"/>
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B21" s="9"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="10"/>
-      <c r="G21" s="11"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="10"/>
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
@@ -1046,12 +1056,12 @@
       <c r="O21" s="3"/>
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B22" s="9"/>
-      <c r="C22" s="10"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="10"/>
-      <c r="G22" s="11"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="10"/>
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
@@ -1062,12 +1072,12 @@
       <c r="O22" s="3"/>
     </row>
     <row r="23" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B23" s="9"/>
-      <c r="C23" s="10"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="10"/>
-      <c r="F23" s="10"/>
-      <c r="G23" s="11"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="10"/>
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
@@ -1078,12 +1088,12 @@
       <c r="O23" s="3"/>
     </row>
     <row r="24" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B24" s="9"/>
-      <c r="C24" s="10"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="10"/>
-      <c r="F24" s="10"/>
-      <c r="G24" s="11"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="10"/>
       <c r="H24" s="3"/>
       <c r="I24" s="3"/>
       <c r="J24" s="3"/>
@@ -1094,12 +1104,12 @@
       <c r="O24" s="3"/>
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B25" s="9"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="10"/>
-      <c r="F25" s="10"/>
-      <c r="G25" s="11"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="10"/>
       <c r="H25" s="3"/>
       <c r="I25" s="3"/>
       <c r="J25" s="3"/>
@@ -1110,12 +1120,12 @@
       <c r="O25" s="3"/>
     </row>
     <row r="26" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B26" s="9"/>
-      <c r="C26" s="10"/>
-      <c r="D26" s="10"/>
-      <c r="E26" s="10"/>
-      <c r="F26" s="10"/>
-      <c r="G26" s="11"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="10"/>
       <c r="H26" s="3"/>
       <c r="I26" s="3"/>
       <c r="J26" s="3"/>
@@ -1126,12 +1136,12 @@
       <c r="O26" s="3"/>
     </row>
     <row r="27" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B27" s="9"/>
-      <c r="C27" s="10"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="10"/>
-      <c r="F27" s="10"/>
-      <c r="G27" s="11"/>
+      <c r="B27" s="8"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="10"/>
       <c r="H27" s="3"/>
       <c r="I27" s="3"/>
       <c r="J27" s="3"/>
@@ -1142,12 +1152,12 @@
       <c r="O27" s="3"/>
     </row>
     <row r="28" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B28" s="9"/>
-      <c r="C28" s="10"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="10"/>
-      <c r="F28" s="10"/>
-      <c r="G28" s="11"/>
+      <c r="B28" s="8"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="10"/>
       <c r="H28" s="3"/>
       <c r="I28" s="3"/>
       <c r="J28" s="3"/>
@@ -1158,12 +1168,12 @@
       <c r="O28" s="3"/>
     </row>
     <row r="29" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B29" s="9"/>
-      <c r="C29" s="10"/>
-      <c r="D29" s="10"/>
-      <c r="E29" s="10"/>
-      <c r="F29" s="10"/>
-      <c r="G29" s="11"/>
+      <c r="B29" s="8"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="10"/>
       <c r="H29" s="3"/>
       <c r="I29" s="3"/>
       <c r="J29" s="3"/>
@@ -1174,12 +1184,12 @@
       <c r="O29" s="3"/>
     </row>
     <row r="30" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B30" s="9"/>
-      <c r="C30" s="10"/>
-      <c r="D30" s="10"/>
-      <c r="E30" s="10"/>
-      <c r="F30" s="10"/>
-      <c r="G30" s="11"/>
+      <c r="B30" s="8"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="10"/>
       <c r="H30" s="3"/>
       <c r="I30" s="3"/>
       <c r="J30" s="3"/>
@@ -1190,12 +1200,12 @@
       <c r="O30" s="3"/>
     </row>
     <row r="31" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B31" s="9"/>
-      <c r="C31" s="10"/>
-      <c r="D31" s="10"/>
-      <c r="E31" s="10"/>
-      <c r="F31" s="10"/>
-      <c r="G31" s="11"/>
+      <c r="B31" s="8"/>
+      <c r="C31" s="9"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="9"/>
+      <c r="G31" s="10"/>
       <c r="H31" s="3"/>
       <c r="I31" s="3"/>
       <c r="J31" s="3"/>
@@ -1206,12 +1216,12 @@
       <c r="O31" s="3"/>
     </row>
     <row r="32" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B32" s="9"/>
-      <c r="C32" s="10"/>
-      <c r="D32" s="10"/>
-      <c r="E32" s="10"/>
-      <c r="F32" s="10"/>
-      <c r="G32" s="11"/>
+      <c r="B32" s="8"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="10"/>
       <c r="H32" s="3"/>
       <c r="I32" s="3"/>
       <c r="J32" s="3"/>
@@ -1222,12 +1232,12 @@
       <c r="O32" s="3"/>
     </row>
     <row r="33" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B33" s="9"/>
-      <c r="C33" s="10"/>
-      <c r="D33" s="10"/>
-      <c r="E33" s="10"/>
-      <c r="F33" s="10"/>
-      <c r="G33" s="11"/>
+      <c r="B33" s="8"/>
+      <c r="C33" s="9"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="10"/>
       <c r="H33" s="3"/>
       <c r="I33" s="3"/>
       <c r="J33" s="3"/>
@@ -1238,12 +1248,12 @@
       <c r="O33" s="3"/>
     </row>
     <row r="34" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B34" s="9"/>
-      <c r="C34" s="10"/>
-      <c r="D34" s="10"/>
-      <c r="E34" s="10"/>
-      <c r="F34" s="10"/>
-      <c r="G34" s="11"/>
+      <c r="B34" s="8"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="9"/>
+      <c r="G34" s="10"/>
       <c r="H34" s="3"/>
       <c r="I34" s="3"/>
       <c r="J34" s="3"/>
@@ -1254,12 +1264,12 @@
       <c r="O34" s="3"/>
     </row>
     <row r="35" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B35" s="9"/>
-      <c r="C35" s="10"/>
-      <c r="D35" s="10"/>
-      <c r="E35" s="10"/>
-      <c r="F35" s="10"/>
-      <c r="G35" s="11"/>
+      <c r="B35" s="8"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="9"/>
+      <c r="G35" s="10"/>
       <c r="H35" s="3"/>
       <c r="I35" s="3"/>
       <c r="J35" s="3"/>
@@ -1270,12 +1280,12 @@
       <c r="O35" s="3"/>
     </row>
     <row r="36" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B36" s="9"/>
-      <c r="C36" s="10"/>
-      <c r="D36" s="10"/>
-      <c r="E36" s="10"/>
-      <c r="F36" s="10"/>
-      <c r="G36" s="11"/>
+      <c r="B36" s="8"/>
+      <c r="C36" s="9"/>
+      <c r="D36" s="9"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="9"/>
+      <c r="G36" s="10"/>
       <c r="H36" s="3"/>
       <c r="I36" s="3"/>
       <c r="J36" s="3"/>
@@ -1286,12 +1296,12 @@
       <c r="O36" s="3"/>
     </row>
     <row r="37" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B37" s="9"/>
-      <c r="C37" s="10"/>
-      <c r="D37" s="10"/>
-      <c r="E37" s="10"/>
-      <c r="F37" s="10"/>
-      <c r="G37" s="11"/>
+      <c r="B37" s="8"/>
+      <c r="C37" s="9"/>
+      <c r="D37" s="9"/>
+      <c r="E37" s="9"/>
+      <c r="F37" s="9"/>
+      <c r="G37" s="10"/>
       <c r="H37" s="3"/>
       <c r="I37" s="3"/>
       <c r="J37" s="3"/>
@@ -1302,12 +1312,12 @@
       <c r="O37" s="3"/>
     </row>
     <row r="38" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B38" s="9"/>
-      <c r="C38" s="10"/>
-      <c r="D38" s="10"/>
-      <c r="E38" s="10"/>
-      <c r="F38" s="10"/>
-      <c r="G38" s="11"/>
+      <c r="B38" s="8"/>
+      <c r="C38" s="9"/>
+      <c r="D38" s="9"/>
+      <c r="E38" s="9"/>
+      <c r="F38" s="9"/>
+      <c r="G38" s="10"/>
       <c r="H38" s="3"/>
       <c r="I38" s="3"/>
       <c r="J38" s="3"/>
@@ -1318,12 +1328,12 @@
       <c r="O38" s="3"/>
     </row>
     <row r="39" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B39" s="9"/>
-      <c r="C39" s="10"/>
-      <c r="D39" s="10"/>
-      <c r="E39" s="10"/>
-      <c r="F39" s="10"/>
-      <c r="G39" s="11"/>
+      <c r="B39" s="8"/>
+      <c r="C39" s="9"/>
+      <c r="D39" s="9"/>
+      <c r="E39" s="9"/>
+      <c r="F39" s="9"/>
+      <c r="G39" s="10"/>
       <c r="H39" s="3"/>
       <c r="I39" s="3"/>
       <c r="J39" s="3"/>
@@ -1334,12 +1344,12 @@
       <c r="O39" s="3"/>
     </row>
     <row r="40" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B40" s="9"/>
-      <c r="C40" s="10"/>
-      <c r="D40" s="10"/>
-      <c r="E40" s="10"/>
-      <c r="F40" s="10"/>
-      <c r="G40" s="11"/>
+      <c r="B40" s="8"/>
+      <c r="C40" s="9"/>
+      <c r="D40" s="9"/>
+      <c r="E40" s="9"/>
+      <c r="F40" s="9"/>
+      <c r="G40" s="10"/>
       <c r="H40" s="3"/>
       <c r="I40" s="3"/>
       <c r="J40" s="3"/>
@@ -1350,12 +1360,12 @@
       <c r="O40" s="3"/>
     </row>
     <row r="41" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B41" s="9"/>
-      <c r="C41" s="10"/>
-      <c r="D41" s="10"/>
-      <c r="E41" s="10"/>
-      <c r="F41" s="10"/>
-      <c r="G41" s="11"/>
+      <c r="B41" s="8"/>
+      <c r="C41" s="9"/>
+      <c r="D41" s="9"/>
+      <c r="E41" s="9"/>
+      <c r="F41" s="9"/>
+      <c r="G41" s="10"/>
       <c r="H41" s="3"/>
       <c r="I41" s="3"/>
       <c r="J41" s="3"/>
@@ -1366,12 +1376,12 @@
       <c r="O41" s="3"/>
     </row>
     <row r="42" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B42" s="9"/>
-      <c r="C42" s="10"/>
-      <c r="D42" s="10"/>
-      <c r="E42" s="10"/>
-      <c r="F42" s="10"/>
-      <c r="G42" s="11"/>
+      <c r="B42" s="8"/>
+      <c r="C42" s="9"/>
+      <c r="D42" s="9"/>
+      <c r="E42" s="9"/>
+      <c r="F42" s="9"/>
+      <c r="G42" s="10"/>
       <c r="H42" s="3"/>
       <c r="I42" s="3"/>
       <c r="J42" s="3"/>
@@ -1382,12 +1392,12 @@
       <c r="O42" s="3"/>
     </row>
     <row r="43" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B43" s="9"/>
-      <c r="C43" s="10"/>
-      <c r="D43" s="10"/>
-      <c r="E43" s="10"/>
-      <c r="F43" s="10"/>
-      <c r="G43" s="11"/>
+      <c r="B43" s="8"/>
+      <c r="C43" s="9"/>
+      <c r="D43" s="9"/>
+      <c r="E43" s="9"/>
+      <c r="F43" s="9"/>
+      <c r="G43" s="10"/>
       <c r="H43" s="3"/>
       <c r="I43" s="3"/>
       <c r="J43" s="3"/>
@@ -1398,12 +1408,12 @@
       <c r="O43" s="3"/>
     </row>
     <row r="44" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B44" s="9"/>
-      <c r="C44" s="10"/>
-      <c r="D44" s="10"/>
-      <c r="E44" s="10"/>
-      <c r="F44" s="10"/>
-      <c r="G44" s="11"/>
+      <c r="B44" s="8"/>
+      <c r="C44" s="9"/>
+      <c r="D44" s="9"/>
+      <c r="E44" s="9"/>
+      <c r="F44" s="9"/>
+      <c r="G44" s="10"/>
       <c r="H44" s="3"/>
       <c r="I44" s="3"/>
       <c r="J44" s="3"/>
@@ -1414,12 +1424,12 @@
       <c r="O44" s="3"/>
     </row>
     <row r="45" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B45" s="9"/>
-      <c r="C45" s="10"/>
-      <c r="D45" s="10"/>
-      <c r="E45" s="10"/>
-      <c r="F45" s="10"/>
-      <c r="G45" s="11"/>
+      <c r="B45" s="8"/>
+      <c r="C45" s="9"/>
+      <c r="D45" s="9"/>
+      <c r="E45" s="9"/>
+      <c r="F45" s="9"/>
+      <c r="G45" s="10"/>
       <c r="H45" s="3"/>
       <c r="I45" s="3"/>
       <c r="J45" s="3"/>
@@ -1430,12 +1440,12 @@
       <c r="O45" s="3"/>
     </row>
     <row r="46" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B46" s="9"/>
-      <c r="C46" s="10"/>
-      <c r="D46" s="10"/>
-      <c r="E46" s="10"/>
-      <c r="F46" s="10"/>
-      <c r="G46" s="11"/>
+      <c r="B46" s="8"/>
+      <c r="C46" s="9"/>
+      <c r="D46" s="9"/>
+      <c r="E46" s="9"/>
+      <c r="F46" s="9"/>
+      <c r="G46" s="10"/>
       <c r="H46" s="3"/>
       <c r="I46" s="3"/>
       <c r="J46" s="3"/>
@@ -1446,12 +1456,12 @@
       <c r="O46" s="3"/>
     </row>
     <row r="47" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B47" s="9"/>
-      <c r="C47" s="10"/>
-      <c r="D47" s="10"/>
-      <c r="E47" s="10"/>
-      <c r="F47" s="10"/>
-      <c r="G47" s="11"/>
+      <c r="B47" s="8"/>
+      <c r="C47" s="9"/>
+      <c r="D47" s="9"/>
+      <c r="E47" s="9"/>
+      <c r="F47" s="9"/>
+      <c r="G47" s="10"/>
       <c r="H47" s="3"/>
       <c r="I47" s="3"/>
       <c r="J47" s="3"/>
@@ -1462,12 +1472,12 @@
       <c r="O47" s="3"/>
     </row>
     <row r="48" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B48" s="9"/>
-      <c r="C48" s="10"/>
-      <c r="D48" s="10"/>
-      <c r="E48" s="10"/>
-      <c r="F48" s="10"/>
-      <c r="G48" s="11"/>
+      <c r="B48" s="8"/>
+      <c r="C48" s="9"/>
+      <c r="D48" s="9"/>
+      <c r="E48" s="9"/>
+      <c r="F48" s="9"/>
+      <c r="G48" s="10"/>
       <c r="H48" s="3"/>
       <c r="I48" s="3"/>
       <c r="J48" s="3"/>
@@ -1478,12 +1488,12 @@
       <c r="O48" s="3"/>
     </row>
     <row r="49" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B49" s="9"/>
-      <c r="C49" s="10"/>
-      <c r="D49" s="10"/>
-      <c r="E49" s="10"/>
-      <c r="F49" s="10"/>
-      <c r="G49" s="11"/>
+      <c r="B49" s="8"/>
+      <c r="C49" s="9"/>
+      <c r="D49" s="9"/>
+      <c r="E49" s="9"/>
+      <c r="F49" s="9"/>
+      <c r="G49" s="10"/>
       <c r="H49" s="3"/>
       <c r="I49" s="3"/>
       <c r="J49" s="3"/>
@@ -1494,12 +1504,12 @@
       <c r="O49" s="3"/>
     </row>
     <row r="50" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B50" s="9"/>
-      <c r="C50" s="10"/>
-      <c r="D50" s="10"/>
-      <c r="E50" s="10"/>
-      <c r="F50" s="10"/>
-      <c r="G50" s="11"/>
+      <c r="B50" s="8"/>
+      <c r="C50" s="9"/>
+      <c r="D50" s="9"/>
+      <c r="E50" s="9"/>
+      <c r="F50" s="9"/>
+      <c r="G50" s="10"/>
       <c r="H50" s="3"/>
       <c r="I50" s="3"/>
       <c r="J50" s="3"/>
@@ -1510,12 +1520,12 @@
       <c r="O50" s="3"/>
     </row>
     <row r="51" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B51" s="9"/>
-      <c r="C51" s="10"/>
-      <c r="D51" s="10"/>
-      <c r="E51" s="10"/>
-      <c r="F51" s="10"/>
-      <c r="G51" s="11"/>
+      <c r="B51" s="8"/>
+      <c r="C51" s="9"/>
+      <c r="D51" s="9"/>
+      <c r="E51" s="9"/>
+      <c r="F51" s="9"/>
+      <c r="G51" s="10"/>
       <c r="H51" s="3"/>
       <c r="I51" s="3"/>
       <c r="J51" s="3"/>
@@ -1526,12 +1536,12 @@
       <c r="O51" s="3"/>
     </row>
     <row r="52" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B52" s="9"/>
-      <c r="C52" s="10"/>
-      <c r="D52" s="10"/>
-      <c r="E52" s="10"/>
-      <c r="F52" s="10"/>
-      <c r="G52" s="11"/>
+      <c r="B52" s="8"/>
+      <c r="C52" s="9"/>
+      <c r="D52" s="9"/>
+      <c r="E52" s="9"/>
+      <c r="F52" s="9"/>
+      <c r="G52" s="10"/>
       <c r="H52" s="3"/>
       <c r="I52" s="3"/>
       <c r="J52" s="3"/>
@@ -1542,12 +1552,12 @@
       <c r="O52" s="3"/>
     </row>
     <row r="53" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B53" s="9"/>
-      <c r="C53" s="10"/>
-      <c r="D53" s="10"/>
-      <c r="E53" s="10"/>
-      <c r="F53" s="10"/>
-      <c r="G53" s="11"/>
+      <c r="B53" s="8"/>
+      <c r="C53" s="9"/>
+      <c r="D53" s="9"/>
+      <c r="E53" s="9"/>
+      <c r="F53" s="9"/>
+      <c r="G53" s="10"/>
       <c r="H53" s="3"/>
       <c r="I53" s="3"/>
       <c r="J53" s="3"/>
@@ -1558,12 +1568,12 @@
       <c r="O53" s="3"/>
     </row>
     <row r="54" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B54" s="9"/>
-      <c r="C54" s="10"/>
-      <c r="D54" s="10"/>
-      <c r="E54" s="10"/>
-      <c r="F54" s="10"/>
-      <c r="G54" s="11"/>
+      <c r="B54" s="8"/>
+      <c r="C54" s="9"/>
+      <c r="D54" s="9"/>
+      <c r="E54" s="9"/>
+      <c r="F54" s="9"/>
+      <c r="G54" s="10"/>
       <c r="H54" s="3"/>
       <c r="I54" s="3"/>
       <c r="J54" s="3"/>
@@ -1574,12 +1584,12 @@
       <c r="O54" s="3"/>
     </row>
     <row r="55" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B55" s="9"/>
-      <c r="C55" s="10"/>
-      <c r="D55" s="10"/>
-      <c r="E55" s="10"/>
-      <c r="F55" s="10"/>
-      <c r="G55" s="11"/>
+      <c r="B55" s="8"/>
+      <c r="C55" s="9"/>
+      <c r="D55" s="9"/>
+      <c r="E55" s="9"/>
+      <c r="F55" s="9"/>
+      <c r="G55" s="10"/>
       <c r="H55" s="3"/>
       <c r="I55" s="3"/>
       <c r="J55" s="3"/>
@@ -1590,12 +1600,12 @@
       <c r="O55" s="3"/>
     </row>
     <row r="56" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B56" s="9"/>
-      <c r="C56" s="10"/>
-      <c r="D56" s="10"/>
-      <c r="E56" s="10"/>
-      <c r="F56" s="10"/>
-      <c r="G56" s="11"/>
+      <c r="B56" s="8"/>
+      <c r="C56" s="9"/>
+      <c r="D56" s="9"/>
+      <c r="E56" s="9"/>
+      <c r="F56" s="9"/>
+      <c r="G56" s="10"/>
       <c r="H56" s="3"/>
       <c r="I56" s="3"/>
       <c r="J56" s="3"/>
@@ -1606,12 +1616,12 @@
       <c r="O56" s="3"/>
     </row>
     <row r="57" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B57" s="9"/>
-      <c r="C57" s="10"/>
-      <c r="D57" s="10"/>
-      <c r="E57" s="10"/>
-      <c r="F57" s="10"/>
-      <c r="G57" s="11"/>
+      <c r="B57" s="8"/>
+      <c r="C57" s="9"/>
+      <c r="D57" s="9"/>
+      <c r="E57" s="9"/>
+      <c r="F57" s="9"/>
+      <c r="G57" s="10"/>
       <c r="H57" s="3"/>
       <c r="I57" s="3"/>
       <c r="J57" s="3"/>
@@ -1622,12 +1632,12 @@
       <c r="O57" s="3"/>
     </row>
     <row r="58" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B58" s="9"/>
-      <c r="C58" s="10"/>
-      <c r="D58" s="10"/>
-      <c r="E58" s="10"/>
-      <c r="F58" s="10"/>
-      <c r="G58" s="11"/>
+      <c r="B58" s="8"/>
+      <c r="C58" s="9"/>
+      <c r="D58" s="9"/>
+      <c r="E58" s="9"/>
+      <c r="F58" s="9"/>
+      <c r="G58" s="10"/>
       <c r="H58" s="3"/>
       <c r="I58" s="3"/>
       <c r="J58" s="3"/>
@@ -1638,12 +1648,12 @@
       <c r="O58" s="3"/>
     </row>
     <row r="59" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B59" s="9"/>
-      <c r="C59" s="10"/>
-      <c r="D59" s="10"/>
-      <c r="E59" s="10"/>
-      <c r="F59" s="10"/>
-      <c r="G59" s="11"/>
+      <c r="B59" s="8"/>
+      <c r="C59" s="9"/>
+      <c r="D59" s="9"/>
+      <c r="E59" s="9"/>
+      <c r="F59" s="9"/>
+      <c r="G59" s="10"/>
       <c r="H59" s="3"/>
       <c r="I59" s="3"/>
       <c r="J59" s="3"/>
@@ -1654,12 +1664,12 @@
       <c r="O59" s="3"/>
     </row>
     <row r="60" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B60" s="9"/>
-      <c r="C60" s="10"/>
-      <c r="D60" s="10"/>
-      <c r="E60" s="10"/>
-      <c r="F60" s="10"/>
-      <c r="G60" s="11"/>
+      <c r="B60" s="8"/>
+      <c r="C60" s="9"/>
+      <c r="D60" s="9"/>
+      <c r="E60" s="9"/>
+      <c r="F60" s="9"/>
+      <c r="G60" s="10"/>
       <c r="H60" s="3"/>
       <c r="I60" s="3"/>
       <c r="J60" s="3"/>
@@ -1670,12 +1680,12 @@
       <c r="O60" s="3"/>
     </row>
     <row r="61" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B61" s="9"/>
-      <c r="C61" s="10"/>
-      <c r="D61" s="10"/>
-      <c r="E61" s="10"/>
-      <c r="F61" s="10"/>
-      <c r="G61" s="11"/>
+      <c r="B61" s="8"/>
+      <c r="C61" s="9"/>
+      <c r="D61" s="9"/>
+      <c r="E61" s="9"/>
+      <c r="F61" s="9"/>
+      <c r="G61" s="10"/>
       <c r="H61" s="3"/>
       <c r="I61" s="3"/>
       <c r="J61" s="3"/>
@@ -1686,12 +1696,12 @@
       <c r="O61" s="3"/>
     </row>
     <row r="62" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B62" s="9"/>
-      <c r="C62" s="10"/>
-      <c r="D62" s="10"/>
-      <c r="E62" s="10"/>
-      <c r="F62" s="10"/>
-      <c r="G62" s="11"/>
+      <c r="B62" s="8"/>
+      <c r="C62" s="9"/>
+      <c r="D62" s="9"/>
+      <c r="E62" s="9"/>
+      <c r="F62" s="9"/>
+      <c r="G62" s="10"/>
       <c r="H62" s="3"/>
       <c r="I62" s="3"/>
       <c r="J62" s="3"/>
@@ -1702,12 +1712,12 @@
       <c r="O62" s="3"/>
     </row>
     <row r="63" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B63" s="9"/>
-      <c r="C63" s="10"/>
-      <c r="D63" s="10"/>
-      <c r="E63" s="10"/>
-      <c r="F63" s="10"/>
-      <c r="G63" s="11"/>
+      <c r="B63" s="8"/>
+      <c r="C63" s="9"/>
+      <c r="D63" s="9"/>
+      <c r="E63" s="9"/>
+      <c r="F63" s="9"/>
+      <c r="G63" s="10"/>
       <c r="H63" s="3"/>
       <c r="I63" s="3"/>
       <c r="J63" s="3"/>
@@ -1718,12 +1728,12 @@
       <c r="O63" s="3"/>
     </row>
     <row r="64" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B64" s="9"/>
-      <c r="C64" s="10"/>
-      <c r="D64" s="10"/>
-      <c r="E64" s="10"/>
-      <c r="F64" s="10"/>
-      <c r="G64" s="11"/>
+      <c r="B64" s="8"/>
+      <c r="C64" s="9"/>
+      <c r="D64" s="9"/>
+      <c r="E64" s="9"/>
+      <c r="F64" s="9"/>
+      <c r="G64" s="10"/>
       <c r="H64" s="3"/>
       <c r="I64" s="3"/>
       <c r="J64" s="3"/>
@@ -1734,12 +1744,12 @@
       <c r="O64" s="3"/>
     </row>
     <row r="65" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B65" s="9"/>
-      <c r="C65" s="10"/>
-      <c r="D65" s="10"/>
-      <c r="E65" s="10"/>
-      <c r="F65" s="10"/>
-      <c r="G65" s="11"/>
+      <c r="B65" s="8"/>
+      <c r="C65" s="9"/>
+      <c r="D65" s="9"/>
+      <c r="E65" s="9"/>
+      <c r="F65" s="9"/>
+      <c r="G65" s="10"/>
       <c r="H65" s="3"/>
       <c r="I65" s="3"/>
       <c r="J65" s="3"/>
@@ -1750,12 +1760,12 @@
       <c r="O65" s="3"/>
     </row>
     <row r="66" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B66" s="9"/>
-      <c r="C66" s="10"/>
-      <c r="D66" s="10"/>
-      <c r="E66" s="10"/>
-      <c r="F66" s="10"/>
-      <c r="G66" s="11"/>
+      <c r="B66" s="8"/>
+      <c r="C66" s="9"/>
+      <c r="D66" s="9"/>
+      <c r="E66" s="9"/>
+      <c r="F66" s="9"/>
+      <c r="G66" s="10"/>
       <c r="H66" s="3"/>
       <c r="I66" s="3"/>
       <c r="J66" s="3"/>
@@ -1766,12 +1776,12 @@
       <c r="O66" s="3"/>
     </row>
     <row r="67" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B67" s="9"/>
-      <c r="C67" s="10"/>
-      <c r="D67" s="10"/>
-      <c r="E67" s="10"/>
-      <c r="F67" s="10"/>
-      <c r="G67" s="11"/>
+      <c r="B67" s="8"/>
+      <c r="C67" s="9"/>
+      <c r="D67" s="9"/>
+      <c r="E67" s="9"/>
+      <c r="F67" s="9"/>
+      <c r="G67" s="10"/>
       <c r="H67" s="3"/>
       <c r="I67" s="3"/>
       <c r="J67" s="3"/>
@@ -1782,12 +1792,12 @@
       <c r="O67" s="3"/>
     </row>
     <row r="68" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B68" s="9"/>
-      <c r="C68" s="10"/>
-      <c r="D68" s="10"/>
-      <c r="E68" s="10"/>
-      <c r="F68" s="10"/>
-      <c r="G68" s="11"/>
+      <c r="B68" s="8"/>
+      <c r="C68" s="9"/>
+      <c r="D68" s="9"/>
+      <c r="E68" s="9"/>
+      <c r="F68" s="9"/>
+      <c r="G68" s="10"/>
       <c r="H68" s="3"/>
       <c r="I68" s="3"/>
       <c r="J68" s="3"/>
@@ -1798,12 +1808,12 @@
       <c r="O68" s="3"/>
     </row>
     <row r="69" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B69" s="9"/>
-      <c r="C69" s="10"/>
-      <c r="D69" s="10"/>
-      <c r="E69" s="10"/>
-      <c r="F69" s="10"/>
-      <c r="G69" s="11"/>
+      <c r="B69" s="8"/>
+      <c r="C69" s="9"/>
+      <c r="D69" s="9"/>
+      <c r="E69" s="9"/>
+      <c r="F69" s="9"/>
+      <c r="G69" s="10"/>
       <c r="H69" s="3"/>
       <c r="I69" s="3"/>
       <c r="J69" s="3"/>
@@ -1814,12 +1824,12 @@
       <c r="O69" s="3"/>
     </row>
     <row r="70" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B70" s="9"/>
-      <c r="C70" s="10"/>
-      <c r="D70" s="10"/>
-      <c r="E70" s="10"/>
-      <c r="F70" s="10"/>
-      <c r="G70" s="11"/>
+      <c r="B70" s="8"/>
+      <c r="C70" s="9"/>
+      <c r="D70" s="9"/>
+      <c r="E70" s="9"/>
+      <c r="F70" s="9"/>
+      <c r="G70" s="10"/>
       <c r="H70" s="3"/>
       <c r="I70" s="3"/>
       <c r="J70" s="3"/>
@@ -1830,12 +1840,12 @@
       <c r="O70" s="3"/>
     </row>
     <row r="71" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B71" s="9"/>
-      <c r="C71" s="10"/>
-      <c r="D71" s="10"/>
-      <c r="E71" s="10"/>
-      <c r="F71" s="10"/>
-      <c r="G71" s="11"/>
+      <c r="B71" s="8"/>
+      <c r="C71" s="9"/>
+      <c r="D71" s="9"/>
+      <c r="E71" s="9"/>
+      <c r="F71" s="9"/>
+      <c r="G71" s="10"/>
       <c r="H71" s="3"/>
       <c r="I71" s="3"/>
       <c r="J71" s="3"/>
@@ -1846,12 +1856,12 @@
       <c r="O71" s="3"/>
     </row>
     <row r="72" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B72" s="9"/>
-      <c r="C72" s="10"/>
-      <c r="D72" s="10"/>
-      <c r="E72" s="10"/>
-      <c r="F72" s="10"/>
-      <c r="G72" s="11"/>
+      <c r="B72" s="8"/>
+      <c r="C72" s="9"/>
+      <c r="D72" s="9"/>
+      <c r="E72" s="9"/>
+      <c r="F72" s="9"/>
+      <c r="G72" s="10"/>
       <c r="H72" s="3"/>
       <c r="I72" s="3"/>
       <c r="J72" s="3"/>
@@ -1862,12 +1872,12 @@
       <c r="O72" s="3"/>
     </row>
     <row r="73" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B73" s="9"/>
-      <c r="C73" s="10"/>
-      <c r="D73" s="10"/>
-      <c r="E73" s="10"/>
-      <c r="F73" s="10"/>
-      <c r="G73" s="11"/>
+      <c r="B73" s="8"/>
+      <c r="C73" s="9"/>
+      <c r="D73" s="9"/>
+      <c r="E73" s="9"/>
+      <c r="F73" s="9"/>
+      <c r="G73" s="10"/>
       <c r="H73" s="3"/>
       <c r="I73" s="3"/>
       <c r="J73" s="3"/>
@@ -1878,12 +1888,12 @@
       <c r="O73" s="3"/>
     </row>
     <row r="74" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B74" s="9"/>
-      <c r="C74" s="10"/>
-      <c r="D74" s="10"/>
-      <c r="E74" s="10"/>
-      <c r="F74" s="10"/>
-      <c r="G74" s="11"/>
+      <c r="B74" s="8"/>
+      <c r="C74" s="9"/>
+      <c r="D74" s="9"/>
+      <c r="E74" s="9"/>
+      <c r="F74" s="9"/>
+      <c r="G74" s="10"/>
       <c r="H74" s="3"/>
       <c r="I74" s="3"/>
       <c r="J74" s="3"/>
@@ -1894,12 +1904,12 @@
       <c r="O74" s="3"/>
     </row>
     <row r="75" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B75" s="9"/>
-      <c r="C75" s="10"/>
-      <c r="D75" s="10"/>
-      <c r="E75" s="10"/>
-      <c r="F75" s="10"/>
-      <c r="G75" s="11"/>
+      <c r="B75" s="8"/>
+      <c r="C75" s="9"/>
+      <c r="D75" s="9"/>
+      <c r="E75" s="9"/>
+      <c r="F75" s="9"/>
+      <c r="G75" s="10"/>
       <c r="H75" s="3"/>
       <c r="I75" s="3"/>
       <c r="J75" s="3"/>
@@ -1910,12 +1920,12 @@
       <c r="O75" s="3"/>
     </row>
     <row r="76" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B76" s="9"/>
-      <c r="C76" s="10"/>
-      <c r="D76" s="10"/>
-      <c r="E76" s="10"/>
-      <c r="F76" s="10"/>
-      <c r="G76" s="11"/>
+      <c r="B76" s="8"/>
+      <c r="C76" s="9"/>
+      <c r="D76" s="9"/>
+      <c r="E76" s="9"/>
+      <c r="F76" s="9"/>
+      <c r="G76" s="10"/>
       <c r="H76" s="3"/>
       <c r="I76" s="3"/>
       <c r="J76" s="3"/>
@@ -1926,12 +1936,12 @@
       <c r="O76" s="3"/>
     </row>
     <row r="77" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B77" s="9"/>
-      <c r="C77" s="10"/>
-      <c r="D77" s="10"/>
-      <c r="E77" s="10"/>
-      <c r="F77" s="10"/>
-      <c r="G77" s="11"/>
+      <c r="B77" s="8"/>
+      <c r="C77" s="9"/>
+      <c r="D77" s="9"/>
+      <c r="E77" s="9"/>
+      <c r="F77" s="9"/>
+      <c r="G77" s="10"/>
       <c r="H77" s="3"/>
       <c r="I77" s="3"/>
       <c r="J77" s="3"/>
@@ -1942,12 +1952,12 @@
       <c r="O77" s="3"/>
     </row>
     <row r="78" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B78" s="9"/>
-      <c r="C78" s="10"/>
-      <c r="D78" s="10"/>
-      <c r="E78" s="10"/>
-      <c r="F78" s="10"/>
-      <c r="G78" s="11"/>
+      <c r="B78" s="8"/>
+      <c r="C78" s="9"/>
+      <c r="D78" s="9"/>
+      <c r="E78" s="9"/>
+      <c r="F78" s="9"/>
+      <c r="G78" s="10"/>
       <c r="H78" s="3"/>
       <c r="I78" s="3"/>
       <c r="J78" s="3"/>
@@ -1958,12 +1968,12 @@
       <c r="O78" s="3"/>
     </row>
     <row r="79" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B79" s="9"/>
-      <c r="C79" s="10"/>
-      <c r="D79" s="10"/>
-      <c r="E79" s="10"/>
-      <c r="F79" s="10"/>
-      <c r="G79" s="11"/>
+      <c r="B79" s="8"/>
+      <c r="C79" s="9"/>
+      <c r="D79" s="9"/>
+      <c r="E79" s="9"/>
+      <c r="F79" s="9"/>
+      <c r="G79" s="10"/>
       <c r="H79" s="3"/>
       <c r="I79" s="3"/>
       <c r="J79" s="3"/>
@@ -1974,12 +1984,12 @@
       <c r="O79" s="3"/>
     </row>
     <row r="80" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B80" s="9"/>
-      <c r="C80" s="10"/>
-      <c r="D80" s="10"/>
-      <c r="E80" s="10"/>
-      <c r="F80" s="10"/>
-      <c r="G80" s="11"/>
+      <c r="B80" s="8"/>
+      <c r="C80" s="9"/>
+      <c r="D80" s="9"/>
+      <c r="E80" s="9"/>
+      <c r="F80" s="9"/>
+      <c r="G80" s="10"/>
       <c r="H80" s="3"/>
       <c r="I80" s="3"/>
       <c r="J80" s="3"/>
@@ -1990,12 +2000,12 @@
       <c r="O80" s="3"/>
     </row>
     <row r="81" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B81" s="9"/>
-      <c r="C81" s="10"/>
-      <c r="D81" s="10"/>
-      <c r="E81" s="10"/>
-      <c r="F81" s="10"/>
-      <c r="G81" s="11"/>
+      <c r="B81" s="8"/>
+      <c r="C81" s="9"/>
+      <c r="D81" s="9"/>
+      <c r="E81" s="9"/>
+      <c r="F81" s="9"/>
+      <c r="G81" s="10"/>
       <c r="H81" s="3"/>
       <c r="I81" s="3"/>
       <c r="J81" s="3"/>
@@ -2006,12 +2016,12 @@
       <c r="O81" s="3"/>
     </row>
     <row r="82" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B82" s="9"/>
-      <c r="C82" s="10"/>
-      <c r="D82" s="10"/>
-      <c r="E82" s="10"/>
-      <c r="F82" s="10"/>
-      <c r="G82" s="11"/>
+      <c r="B82" s="8"/>
+      <c r="C82" s="9"/>
+      <c r="D82" s="9"/>
+      <c r="E82" s="9"/>
+      <c r="F82" s="9"/>
+      <c r="G82" s="10"/>
       <c r="H82" s="3"/>
       <c r="I82" s="3"/>
       <c r="J82" s="3"/>
@@ -2022,12 +2032,12 @@
       <c r="O82" s="3"/>
     </row>
     <row r="83" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B83" s="9"/>
-      <c r="C83" s="10"/>
-      <c r="D83" s="10"/>
-      <c r="E83" s="10"/>
-      <c r="F83" s="10"/>
-      <c r="G83" s="11"/>
+      <c r="B83" s="8"/>
+      <c r="C83" s="9"/>
+      <c r="D83" s="9"/>
+      <c r="E83" s="9"/>
+      <c r="F83" s="9"/>
+      <c r="G83" s="10"/>
       <c r="H83" s="3"/>
       <c r="I83" s="3"/>
       <c r="J83" s="3"/>
@@ -2038,12 +2048,12 @@
       <c r="O83" s="3"/>
     </row>
     <row r="84" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B84" s="9"/>
-      <c r="C84" s="10"/>
-      <c r="D84" s="10"/>
-      <c r="E84" s="10"/>
-      <c r="F84" s="10"/>
-      <c r="G84" s="11"/>
+      <c r="B84" s="8"/>
+      <c r="C84" s="9"/>
+      <c r="D84" s="9"/>
+      <c r="E84" s="9"/>
+      <c r="F84" s="9"/>
+      <c r="G84" s="10"/>
       <c r="H84" s="3"/>
       <c r="I84" s="3"/>
       <c r="J84" s="3"/>
@@ -2054,12 +2064,12 @@
       <c r="O84" s="3"/>
     </row>
     <row r="85" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B85" s="9"/>
-      <c r="C85" s="10"/>
-      <c r="D85" s="10"/>
-      <c r="E85" s="10"/>
-      <c r="F85" s="10"/>
-      <c r="G85" s="11"/>
+      <c r="B85" s="8"/>
+      <c r="C85" s="9"/>
+      <c r="D85" s="9"/>
+      <c r="E85" s="9"/>
+      <c r="F85" s="9"/>
+      <c r="G85" s="10"/>
       <c r="H85" s="3"/>
       <c r="I85" s="3"/>
       <c r="J85" s="3"/>
@@ -2070,12 +2080,12 @@
       <c r="O85" s="3"/>
     </row>
     <row r="86" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B86" s="9"/>
-      <c r="C86" s="10"/>
-      <c r="D86" s="10"/>
-      <c r="E86" s="10"/>
-      <c r="F86" s="10"/>
-      <c r="G86" s="11"/>
+      <c r="B86" s="8"/>
+      <c r="C86" s="9"/>
+      <c r="D86" s="9"/>
+      <c r="E86" s="9"/>
+      <c r="F86" s="9"/>
+      <c r="G86" s="10"/>
       <c r="H86" s="3"/>
       <c r="I86" s="3"/>
       <c r="J86" s="3"/>
@@ -2086,12 +2096,12 @@
       <c r="O86" s="3"/>
     </row>
     <row r="87" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B87" s="9"/>
-      <c r="C87" s="10"/>
-      <c r="D87" s="10"/>
-      <c r="E87" s="10"/>
-      <c r="F87" s="10"/>
-      <c r="G87" s="11"/>
+      <c r="B87" s="8"/>
+      <c r="C87" s="9"/>
+      <c r="D87" s="9"/>
+      <c r="E87" s="9"/>
+      <c r="F87" s="9"/>
+      <c r="G87" s="10"/>
       <c r="H87" s="3"/>
       <c r="I87" s="3"/>
       <c r="J87" s="3"/>
@@ -2102,12 +2112,12 @@
       <c r="O87" s="3"/>
     </row>
     <row r="88" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B88" s="9"/>
-      <c r="C88" s="10"/>
-      <c r="D88" s="10"/>
-      <c r="E88" s="10"/>
-      <c r="F88" s="10"/>
-      <c r="G88" s="11"/>
+      <c r="B88" s="8"/>
+      <c r="C88" s="9"/>
+      <c r="D88" s="9"/>
+      <c r="E88" s="9"/>
+      <c r="F88" s="9"/>
+      <c r="G88" s="10"/>
       <c r="H88" s="3"/>
       <c r="I88" s="3"/>
       <c r="J88" s="3"/>
@@ -2118,12 +2128,12 @@
       <c r="O88" s="3"/>
     </row>
     <row r="89" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B89" s="9"/>
-      <c r="C89" s="10"/>
-      <c r="D89" s="10"/>
-      <c r="E89" s="10"/>
-      <c r="F89" s="10"/>
-      <c r="G89" s="11"/>
+      <c r="B89" s="8"/>
+      <c r="C89" s="9"/>
+      <c r="D89" s="9"/>
+      <c r="E89" s="9"/>
+      <c r="F89" s="9"/>
+      <c r="G89" s="10"/>
       <c r="H89" s="3"/>
       <c r="I89" s="3"/>
       <c r="J89" s="3"/>
@@ -2134,12 +2144,12 @@
       <c r="O89" s="3"/>
     </row>
     <row r="90" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B90" s="9"/>
-      <c r="C90" s="10"/>
-      <c r="D90" s="10"/>
-      <c r="E90" s="10"/>
-      <c r="F90" s="10"/>
-      <c r="G90" s="11"/>
+      <c r="B90" s="8"/>
+      <c r="C90" s="9"/>
+      <c r="D90" s="9"/>
+      <c r="E90" s="9"/>
+      <c r="F90" s="9"/>
+      <c r="G90" s="10"/>
       <c r="H90" s="3"/>
       <c r="I90" s="3"/>
       <c r="J90" s="3"/>
@@ -2150,12 +2160,12 @@
       <c r="O90" s="3"/>
     </row>
     <row r="91" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B91" s="9"/>
-      <c r="C91" s="10"/>
-      <c r="D91" s="10"/>
-      <c r="E91" s="10"/>
-      <c r="F91" s="10"/>
-      <c r="G91" s="11"/>
+      <c r="B91" s="8"/>
+      <c r="C91" s="9"/>
+      <c r="D91" s="9"/>
+      <c r="E91" s="9"/>
+      <c r="F91" s="9"/>
+      <c r="G91" s="10"/>
       <c r="H91" s="3"/>
       <c r="I91" s="3"/>
       <c r="J91" s="3"/>
@@ -2166,12 +2176,12 @@
       <c r="O91" s="3"/>
     </row>
     <row r="92" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B92" s="9"/>
-      <c r="C92" s="10"/>
-      <c r="D92" s="10"/>
-      <c r="E92" s="10"/>
-      <c r="F92" s="10"/>
-      <c r="G92" s="11"/>
+      <c r="B92" s="8"/>
+      <c r="C92" s="9"/>
+      <c r="D92" s="9"/>
+      <c r="E92" s="9"/>
+      <c r="F92" s="9"/>
+      <c r="G92" s="10"/>
       <c r="H92" s="3"/>
       <c r="I92" s="3"/>
       <c r="J92" s="3"/>
@@ -2182,12 +2192,12 @@
       <c r="O92" s="3"/>
     </row>
     <row r="93" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B93" s="9"/>
-      <c r="C93" s="10"/>
-      <c r="D93" s="10"/>
-      <c r="E93" s="10"/>
-      <c r="F93" s="10"/>
-      <c r="G93" s="11"/>
+      <c r="B93" s="8"/>
+      <c r="C93" s="9"/>
+      <c r="D93" s="9"/>
+      <c r="E93" s="9"/>
+      <c r="F93" s="9"/>
+      <c r="G93" s="10"/>
       <c r="H93" s="3"/>
       <c r="I93" s="3"/>
       <c r="J93" s="3"/>
@@ -2198,12 +2208,12 @@
       <c r="O93" s="3"/>
     </row>
     <row r="94" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B94" s="9"/>
-      <c r="C94" s="10"/>
-      <c r="D94" s="10"/>
-      <c r="E94" s="10"/>
-      <c r="F94" s="10"/>
-      <c r="G94" s="11"/>
+      <c r="B94" s="8"/>
+      <c r="C94" s="9"/>
+      <c r="D94" s="9"/>
+      <c r="E94" s="9"/>
+      <c r="F94" s="9"/>
+      <c r="G94" s="10"/>
       <c r="H94" s="3"/>
       <c r="I94" s="3"/>
       <c r="J94" s="3"/>
@@ -2214,12 +2224,12 @@
       <c r="O94" s="3"/>
     </row>
     <row r="95" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B95" s="9"/>
-      <c r="C95" s="10"/>
-      <c r="D95" s="10"/>
-      <c r="E95" s="10"/>
-      <c r="F95" s="10"/>
-      <c r="G95" s="11"/>
+      <c r="B95" s="8"/>
+      <c r="C95" s="9"/>
+      <c r="D95" s="9"/>
+      <c r="E95" s="9"/>
+      <c r="F95" s="9"/>
+      <c r="G95" s="10"/>
       <c r="H95" s="3"/>
       <c r="I95" s="3"/>
       <c r="J95" s="3"/>
@@ -2230,12 +2240,12 @@
       <c r="O95" s="3"/>
     </row>
     <row r="96" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B96" s="9"/>
-      <c r="C96" s="10"/>
-      <c r="D96" s="10"/>
-      <c r="E96" s="10"/>
-      <c r="F96" s="10"/>
-      <c r="G96" s="11"/>
+      <c r="B96" s="8"/>
+      <c r="C96" s="9"/>
+      <c r="D96" s="9"/>
+      <c r="E96" s="9"/>
+      <c r="F96" s="9"/>
+      <c r="G96" s="10"/>
       <c r="H96" s="3"/>
       <c r="I96" s="3"/>
       <c r="J96" s="3"/>
@@ -2246,12 +2256,12 @@
       <c r="O96" s="3"/>
     </row>
     <row r="97" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B97" s="9"/>
-      <c r="C97" s="10"/>
-      <c r="D97" s="10"/>
-      <c r="E97" s="10"/>
-      <c r="F97" s="10"/>
-      <c r="G97" s="11"/>
+      <c r="B97" s="8"/>
+      <c r="C97" s="9"/>
+      <c r="D97" s="9"/>
+      <c r="E97" s="9"/>
+      <c r="F97" s="9"/>
+      <c r="G97" s="10"/>
       <c r="H97" s="3"/>
       <c r="I97" s="3"/>
       <c r="J97" s="3"/>
@@ -2262,12 +2272,12 @@
       <c r="O97" s="3"/>
     </row>
     <row r="98" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B98" s="9"/>
-      <c r="C98" s="10"/>
-      <c r="D98" s="10"/>
-      <c r="E98" s="10"/>
-      <c r="F98" s="10"/>
-      <c r="G98" s="11"/>
+      <c r="B98" s="8"/>
+      <c r="C98" s="9"/>
+      <c r="D98" s="9"/>
+      <c r="E98" s="9"/>
+      <c r="F98" s="9"/>
+      <c r="G98" s="10"/>
       <c r="H98" s="3"/>
       <c r="I98" s="3"/>
       <c r="J98" s="3"/>
@@ -2278,12 +2288,12 @@
       <c r="O98" s="3"/>
     </row>
     <row r="99" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B99" s="9"/>
-      <c r="C99" s="10"/>
-      <c r="D99" s="10"/>
-      <c r="E99" s="10"/>
-      <c r="F99" s="10"/>
-      <c r="G99" s="11"/>
+      <c r="B99" s="8"/>
+      <c r="C99" s="9"/>
+      <c r="D99" s="9"/>
+      <c r="E99" s="9"/>
+      <c r="F99" s="9"/>
+      <c r="G99" s="10"/>
       <c r="H99" s="3"/>
       <c r="I99" s="3"/>
       <c r="J99" s="3"/>
@@ -2294,12 +2304,12 @@
       <c r="O99" s="3"/>
     </row>
     <row r="100" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B100" s="9"/>
-      <c r="C100" s="10"/>
-      <c r="D100" s="10"/>
-      <c r="E100" s="10"/>
-      <c r="F100" s="10"/>
-      <c r="G100" s="11"/>
+      <c r="B100" s="8"/>
+      <c r="C100" s="9"/>
+      <c r="D100" s="9"/>
+      <c r="E100" s="9"/>
+      <c r="F100" s="9"/>
+      <c r="G100" s="10"/>
       <c r="H100" s="3"/>
       <c r="I100" s="3"/>
       <c r="J100" s="3"/>
@@ -2310,12 +2320,12 @@
       <c r="O100" s="3"/>
     </row>
     <row r="101" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B101" s="9"/>
-      <c r="C101" s="10"/>
-      <c r="D101" s="10"/>
-      <c r="E101" s="10"/>
-      <c r="F101" s="10"/>
-      <c r="G101" s="11"/>
+      <c r="B101" s="8"/>
+      <c r="C101" s="9"/>
+      <c r="D101" s="9"/>
+      <c r="E101" s="9"/>
+      <c r="F101" s="9"/>
+      <c r="G101" s="10"/>
       <c r="H101" s="3"/>
       <c r="I101" s="3"/>
       <c r="J101" s="3"/>
@@ -2326,12 +2336,12 @@
       <c r="O101" s="3"/>
     </row>
     <row r="102" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B102" s="9"/>
-      <c r="C102" s="10"/>
-      <c r="D102" s="10"/>
-      <c r="E102" s="10"/>
-      <c r="F102" s="10"/>
-      <c r="G102" s="11"/>
+      <c r="B102" s="8"/>
+      <c r="C102" s="9"/>
+      <c r="D102" s="9"/>
+      <c r="E102" s="9"/>
+      <c r="F102" s="9"/>
+      <c r="G102" s="10"/>
       <c r="H102" s="3"/>
       <c r="I102" s="3"/>
       <c r="J102" s="3"/>
@@ -2342,12 +2352,12 @@
       <c r="O102" s="3"/>
     </row>
     <row r="103" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B103" s="9"/>
-      <c r="C103" s="10"/>
-      <c r="D103" s="10"/>
-      <c r="E103" s="10"/>
-      <c r="F103" s="10"/>
-      <c r="G103" s="11"/>
+      <c r="B103" s="8"/>
+      <c r="C103" s="9"/>
+      <c r="D103" s="9"/>
+      <c r="E103" s="9"/>
+      <c r="F103" s="9"/>
+      <c r="G103" s="10"/>
       <c r="H103" s="3"/>
       <c r="I103" s="3"/>
       <c r="J103" s="3"/>
@@ -2358,12 +2368,12 @@
       <c r="O103" s="3"/>
     </row>
     <row r="104" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B104" s="9"/>
-      <c r="C104" s="10"/>
-      <c r="D104" s="10"/>
-      <c r="E104" s="10"/>
-      <c r="F104" s="10"/>
-      <c r="G104" s="11"/>
+      <c r="B104" s="8"/>
+      <c r="C104" s="9"/>
+      <c r="D104" s="9"/>
+      <c r="E104" s="9"/>
+      <c r="F104" s="9"/>
+      <c r="G104" s="10"/>
       <c r="H104" s="3"/>
       <c r="I104" s="3"/>
       <c r="J104" s="3"/>
@@ -2374,12 +2384,12 @@
       <c r="O104" s="3"/>
     </row>
     <row r="105" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B105" s="9"/>
-      <c r="C105" s="10"/>
-      <c r="D105" s="10"/>
-      <c r="E105" s="10"/>
-      <c r="F105" s="10"/>
-      <c r="G105" s="11"/>
+      <c r="B105" s="8"/>
+      <c r="C105" s="9"/>
+      <c r="D105" s="9"/>
+      <c r="E105" s="9"/>
+      <c r="F105" s="9"/>
+      <c r="G105" s="10"/>
       <c r="H105" s="3"/>
       <c r="I105" s="3"/>
       <c r="J105" s="3"/>
@@ -2390,12 +2400,12 @@
       <c r="O105" s="3"/>
     </row>
     <row r="106" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B106" s="9"/>
-      <c r="C106" s="10"/>
-      <c r="D106" s="10"/>
-      <c r="E106" s="10"/>
-      <c r="F106" s="10"/>
-      <c r="G106" s="11"/>
+      <c r="B106" s="8"/>
+      <c r="C106" s="9"/>
+      <c r="D106" s="9"/>
+      <c r="E106" s="9"/>
+      <c r="F106" s="9"/>
+      <c r="G106" s="10"/>
       <c r="H106" s="3"/>
       <c r="I106" s="3"/>
       <c r="J106" s="3"/>
@@ -2406,12 +2416,12 @@
       <c r="O106" s="3"/>
     </row>
     <row r="107" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B107" s="9"/>
-      <c r="C107" s="10"/>
-      <c r="D107" s="10"/>
-      <c r="E107" s="10"/>
-      <c r="F107" s="10"/>
-      <c r="G107" s="11"/>
+      <c r="B107" s="8"/>
+      <c r="C107" s="9"/>
+      <c r="D107" s="9"/>
+      <c r="E107" s="9"/>
+      <c r="F107" s="9"/>
+      <c r="G107" s="10"/>
       <c r="H107" s="3"/>
       <c r="I107" s="3"/>
       <c r="J107" s="3"/>
@@ -2422,12 +2432,12 @@
       <c r="O107" s="3"/>
     </row>
     <row r="108" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B108" s="9"/>
-      <c r="C108" s="10"/>
-      <c r="D108" s="10"/>
-      <c r="E108" s="10"/>
-      <c r="F108" s="10"/>
-      <c r="G108" s="11"/>
+      <c r="B108" s="8"/>
+      <c r="C108" s="9"/>
+      <c r="D108" s="9"/>
+      <c r="E108" s="9"/>
+      <c r="F108" s="9"/>
+      <c r="G108" s="10"/>
       <c r="H108" s="3"/>
       <c r="I108" s="3"/>
       <c r="J108" s="3"/>
@@ -2438,12 +2448,12 @@
       <c r="O108" s="3"/>
     </row>
     <row r="109" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B109" s="9"/>
-      <c r="C109" s="10"/>
-      <c r="D109" s="10"/>
-      <c r="E109" s="10"/>
-      <c r="F109" s="10"/>
-      <c r="G109" s="11"/>
+      <c r="B109" s="8"/>
+      <c r="C109" s="9"/>
+      <c r="D109" s="9"/>
+      <c r="E109" s="9"/>
+      <c r="F109" s="9"/>
+      <c r="G109" s="10"/>
       <c r="H109" s="3"/>
       <c r="I109" s="3"/>
       <c r="J109" s="3"/>
@@ -2454,12 +2464,12 @@
       <c r="O109" s="3"/>
     </row>
     <row r="110" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B110" s="9"/>
-      <c r="C110" s="10"/>
-      <c r="D110" s="10"/>
-      <c r="E110" s="10"/>
-      <c r="F110" s="10"/>
-      <c r="G110" s="11"/>
+      <c r="B110" s="8"/>
+      <c r="C110" s="9"/>
+      <c r="D110" s="9"/>
+      <c r="E110" s="9"/>
+      <c r="F110" s="9"/>
+      <c r="G110" s="10"/>
       <c r="H110" s="3"/>
       <c r="I110" s="3"/>
       <c r="J110" s="3"/>
@@ -2470,12 +2480,12 @@
       <c r="O110" s="3"/>
     </row>
     <row r="111" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B111" s="9"/>
-      <c r="C111" s="10"/>
-      <c r="D111" s="10"/>
-      <c r="E111" s="10"/>
-      <c r="F111" s="10"/>
-      <c r="G111" s="11"/>
+      <c r="B111" s="8"/>
+      <c r="C111" s="9"/>
+      <c r="D111" s="9"/>
+      <c r="E111" s="9"/>
+      <c r="F111" s="9"/>
+      <c r="G111" s="10"/>
       <c r="H111" s="3"/>
       <c r="I111" s="3"/>
       <c r="J111" s="3"/>
@@ -2486,12 +2496,12 @@
       <c r="O111" s="3"/>
     </row>
     <row r="112" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B112" s="9"/>
-      <c r="C112" s="10"/>
-      <c r="D112" s="10"/>
-      <c r="E112" s="10"/>
-      <c r="F112" s="10"/>
-      <c r="G112" s="11"/>
+      <c r="B112" s="8"/>
+      <c r="C112" s="9"/>
+      <c r="D112" s="9"/>
+      <c r="E112" s="9"/>
+      <c r="F112" s="9"/>
+      <c r="G112" s="10"/>
       <c r="H112" s="3"/>
       <c r="I112" s="3"/>
       <c r="J112" s="3"/>
@@ -2502,12 +2512,12 @@
       <c r="O112" s="3"/>
     </row>
     <row r="113" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B113" s="9"/>
-      <c r="C113" s="10"/>
-      <c r="D113" s="10"/>
-      <c r="E113" s="10"/>
-      <c r="F113" s="10"/>
-      <c r="G113" s="11"/>
+      <c r="B113" s="8"/>
+      <c r="C113" s="9"/>
+      <c r="D113" s="9"/>
+      <c r="E113" s="9"/>
+      <c r="F113" s="9"/>
+      <c r="G113" s="10"/>
       <c r="H113" s="3"/>
       <c r="I113" s="3"/>
       <c r="J113" s="3"/>
@@ -2518,12 +2528,12 @@
       <c r="O113" s="3"/>
     </row>
     <row r="114" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B114" s="9"/>
-      <c r="C114" s="10"/>
-      <c r="D114" s="10"/>
-      <c r="E114" s="10"/>
-      <c r="F114" s="10"/>
-      <c r="G114" s="11"/>
+      <c r="B114" s="8"/>
+      <c r="C114" s="9"/>
+      <c r="D114" s="9"/>
+      <c r="E114" s="9"/>
+      <c r="F114" s="9"/>
+      <c r="G114" s="10"/>
       <c r="H114" s="3"/>
       <c r="I114" s="3"/>
       <c r="J114" s="3"/>
@@ -2534,12 +2544,12 @@
       <c r="O114" s="3"/>
     </row>
     <row r="115" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B115" s="9"/>
-      <c r="C115" s="10"/>
-      <c r="D115" s="10"/>
-      <c r="E115" s="10"/>
-      <c r="F115" s="10"/>
-      <c r="G115" s="11"/>
+      <c r="B115" s="8"/>
+      <c r="C115" s="9"/>
+      <c r="D115" s="9"/>
+      <c r="E115" s="9"/>
+      <c r="F115" s="9"/>
+      <c r="G115" s="10"/>
       <c r="H115" s="3"/>
       <c r="I115" s="3"/>
       <c r="J115" s="3"/>
@@ -2550,12 +2560,12 @@
       <c r="O115" s="3"/>
     </row>
     <row r="116" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B116" s="9"/>
-      <c r="C116" s="10"/>
-      <c r="D116" s="10"/>
-      <c r="E116" s="10"/>
-      <c r="F116" s="10"/>
-      <c r="G116" s="11"/>
+      <c r="B116" s="8"/>
+      <c r="C116" s="9"/>
+      <c r="D116" s="9"/>
+      <c r="E116" s="9"/>
+      <c r="F116" s="9"/>
+      <c r="G116" s="10"/>
       <c r="H116" s="3"/>
       <c r="I116" s="3"/>
       <c r="J116" s="3"/>
@@ -2566,12 +2576,12 @@
       <c r="O116" s="3"/>
     </row>
     <row r="117" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B117" s="9"/>
-      <c r="C117" s="10"/>
-      <c r="D117" s="10"/>
-      <c r="E117" s="10"/>
-      <c r="F117" s="10"/>
-      <c r="G117" s="11"/>
+      <c r="B117" s="8"/>
+      <c r="C117" s="9"/>
+      <c r="D117" s="9"/>
+      <c r="E117" s="9"/>
+      <c r="F117" s="9"/>
+      <c r="G117" s="10"/>
       <c r="H117" s="3"/>
       <c r="I117" s="3"/>
       <c r="J117" s="3"/>
@@ -2582,12 +2592,12 @@
       <c r="O117" s="3"/>
     </row>
     <row r="118" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B118" s="9"/>
-      <c r="C118" s="10"/>
-      <c r="D118" s="10"/>
-      <c r="E118" s="10"/>
-      <c r="F118" s="10"/>
-      <c r="G118" s="11"/>
+      <c r="B118" s="8"/>
+      <c r="C118" s="9"/>
+      <c r="D118" s="9"/>
+      <c r="E118" s="9"/>
+      <c r="F118" s="9"/>
+      <c r="G118" s="10"/>
       <c r="H118" s="3"/>
       <c r="I118" s="3"/>
       <c r="J118" s="3"/>
@@ -2598,12 +2608,12 @@
       <c r="O118" s="3"/>
     </row>
     <row r="119" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B119" s="9"/>
-      <c r="C119" s="10"/>
-      <c r="D119" s="10"/>
-      <c r="E119" s="10"/>
-      <c r="F119" s="10"/>
-      <c r="G119" s="11"/>
+      <c r="B119" s="8"/>
+      <c r="C119" s="9"/>
+      <c r="D119" s="9"/>
+      <c r="E119" s="9"/>
+      <c r="F119" s="9"/>
+      <c r="G119" s="10"/>
       <c r="H119" s="3"/>
       <c r="I119" s="3"/>
       <c r="J119" s="3"/>
@@ -2614,12 +2624,12 @@
       <c r="O119" s="3"/>
     </row>
     <row r="120" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B120" s="9"/>
-      <c r="C120" s="10"/>
-      <c r="D120" s="10"/>
-      <c r="E120" s="10"/>
-      <c r="F120" s="10"/>
-      <c r="G120" s="11"/>
+      <c r="B120" s="8"/>
+      <c r="C120" s="9"/>
+      <c r="D120" s="9"/>
+      <c r="E120" s="9"/>
+      <c r="F120" s="9"/>
+      <c r="G120" s="10"/>
       <c r="H120" s="3"/>
       <c r="I120" s="3"/>
       <c r="J120" s="3"/>
@@ -2630,12 +2640,12 @@
       <c r="O120" s="3"/>
     </row>
     <row r="121" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B121" s="9"/>
-      <c r="C121" s="10"/>
-      <c r="D121" s="10"/>
-      <c r="E121" s="10"/>
-      <c r="F121" s="10"/>
-      <c r="G121" s="11"/>
+      <c r="B121" s="8"/>
+      <c r="C121" s="9"/>
+      <c r="D121" s="9"/>
+      <c r="E121" s="9"/>
+      <c r="F121" s="9"/>
+      <c r="G121" s="10"/>
       <c r="H121" s="3"/>
       <c r="I121" s="3"/>
       <c r="J121" s="3"/>
@@ -2646,12 +2656,12 @@
       <c r="O121" s="3"/>
     </row>
     <row r="122" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B122" s="9"/>
-      <c r="C122" s="10"/>
-      <c r="D122" s="10"/>
-      <c r="E122" s="10"/>
-      <c r="F122" s="10"/>
-      <c r="G122" s="11"/>
+      <c r="B122" s="8"/>
+      <c r="C122" s="9"/>
+      <c r="D122" s="9"/>
+      <c r="E122" s="9"/>
+      <c r="F122" s="9"/>
+      <c r="G122" s="10"/>
       <c r="H122" s="3"/>
       <c r="I122" s="3"/>
       <c r="J122" s="3"/>
@@ -2662,12 +2672,12 @@
       <c r="O122" s="3"/>
     </row>
     <row r="123" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B123" s="9"/>
-      <c r="C123" s="10"/>
-      <c r="D123" s="10"/>
-      <c r="E123" s="10"/>
-      <c r="F123" s="10"/>
-      <c r="G123" s="11"/>
+      <c r="B123" s="8"/>
+      <c r="C123" s="9"/>
+      <c r="D123" s="9"/>
+      <c r="E123" s="9"/>
+      <c r="F123" s="9"/>
+      <c r="G123" s="10"/>
       <c r="H123" s="3"/>
       <c r="I123" s="3"/>
       <c r="J123" s="3"/>
@@ -2678,12 +2688,12 @@
       <c r="O123" s="3"/>
     </row>
     <row r="124" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B124" s="9"/>
-      <c r="C124" s="10"/>
-      <c r="D124" s="10"/>
-      <c r="E124" s="10"/>
-      <c r="F124" s="10"/>
-      <c r="G124" s="11"/>
+      <c r="B124" s="8"/>
+      <c r="C124" s="9"/>
+      <c r="D124" s="9"/>
+      <c r="E124" s="9"/>
+      <c r="F124" s="9"/>
+      <c r="G124" s="10"/>
       <c r="H124" s="3"/>
       <c r="I124" s="3"/>
       <c r="J124" s="3"/>
@@ -2694,12 +2704,12 @@
       <c r="O124" s="3"/>
     </row>
     <row r="125" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B125" s="9"/>
-      <c r="C125" s="10"/>
-      <c r="D125" s="10"/>
-      <c r="E125" s="10"/>
-      <c r="F125" s="10"/>
-      <c r="G125" s="11"/>
+      <c r="B125" s="8"/>
+      <c r="C125" s="9"/>
+      <c r="D125" s="9"/>
+      <c r="E125" s="9"/>
+      <c r="F125" s="9"/>
+      <c r="G125" s="10"/>
       <c r="H125" s="3"/>
       <c r="I125" s="3"/>
       <c r="J125" s="3"/>
@@ -2710,12 +2720,12 @@
       <c r="O125" s="3"/>
     </row>
     <row r="126" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B126" s="9"/>
-      <c r="C126" s="10"/>
-      <c r="D126" s="10"/>
-      <c r="E126" s="10"/>
-      <c r="F126" s="10"/>
-      <c r="G126" s="11"/>
+      <c r="B126" s="8"/>
+      <c r="C126" s="9"/>
+      <c r="D126" s="9"/>
+      <c r="E126" s="9"/>
+      <c r="F126" s="9"/>
+      <c r="G126" s="10"/>
       <c r="H126" s="3"/>
       <c r="I126" s="3"/>
       <c r="J126" s="3"/>
@@ -2726,12 +2736,12 @@
       <c r="O126" s="3"/>
     </row>
     <row r="127" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B127" s="9"/>
-      <c r="C127" s="10"/>
-      <c r="D127" s="10"/>
-      <c r="E127" s="10"/>
-      <c r="F127" s="10"/>
-      <c r="G127" s="11"/>
+      <c r="B127" s="8"/>
+      <c r="C127" s="9"/>
+      <c r="D127" s="9"/>
+      <c r="E127" s="9"/>
+      <c r="F127" s="9"/>
+      <c r="G127" s="10"/>
       <c r="H127" s="3"/>
       <c r="I127" s="3"/>
       <c r="J127" s="3"/>
@@ -2742,12 +2752,12 @@
       <c r="O127" s="3"/>
     </row>
     <row r="128" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B128" s="9"/>
-      <c r="C128" s="10"/>
-      <c r="D128" s="10"/>
-      <c r="E128" s="10"/>
-      <c r="F128" s="10"/>
-      <c r="G128" s="11"/>
+      <c r="B128" s="8"/>
+      <c r="C128" s="9"/>
+      <c r="D128" s="9"/>
+      <c r="E128" s="9"/>
+      <c r="F128" s="9"/>
+      <c r="G128" s="10"/>
       <c r="H128" s="3"/>
       <c r="I128" s="3"/>
       <c r="J128" s="3"/>
@@ -2758,12 +2768,12 @@
       <c r="O128" s="3"/>
     </row>
     <row r="129" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B129" s="9"/>
-      <c r="C129" s="10"/>
-      <c r="D129" s="10"/>
-      <c r="E129" s="10"/>
-      <c r="F129" s="10"/>
-      <c r="G129" s="11"/>
+      <c r="B129" s="8"/>
+      <c r="C129" s="9"/>
+      <c r="D129" s="9"/>
+      <c r="E129" s="9"/>
+      <c r="F129" s="9"/>
+      <c r="G129" s="10"/>
       <c r="H129" s="3"/>
       <c r="I129" s="3"/>
       <c r="J129" s="3"/>
@@ -2774,12 +2784,12 @@
       <c r="O129" s="3"/>
     </row>
     <row r="130" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B130" s="9"/>
-      <c r="C130" s="10"/>
-      <c r="D130" s="10"/>
-      <c r="E130" s="10"/>
-      <c r="F130" s="10"/>
-      <c r="G130" s="11"/>
+      <c r="B130" s="8"/>
+      <c r="C130" s="9"/>
+      <c r="D130" s="9"/>
+      <c r="E130" s="9"/>
+      <c r="F130" s="9"/>
+      <c r="G130" s="10"/>
       <c r="H130" s="3"/>
       <c r="I130" s="3"/>
       <c r="J130" s="3"/>
@@ -2790,12 +2800,12 @@
       <c r="O130" s="3"/>
     </row>
     <row r="131" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B131" s="9"/>
-      <c r="C131" s="10"/>
-      <c r="D131" s="10"/>
-      <c r="E131" s="10"/>
-      <c r="F131" s="10"/>
-      <c r="G131" s="11"/>
+      <c r="B131" s="8"/>
+      <c r="C131" s="9"/>
+      <c r="D131" s="9"/>
+      <c r="E131" s="9"/>
+      <c r="F131" s="9"/>
+      <c r="G131" s="10"/>
       <c r="H131" s="3"/>
       <c r="I131" s="3"/>
       <c r="J131" s="3"/>
@@ -2806,12 +2816,12 @@
       <c r="O131" s="3"/>
     </row>
     <row r="132" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B132" s="9"/>
-      <c r="C132" s="10"/>
-      <c r="D132" s="10"/>
-      <c r="E132" s="10"/>
-      <c r="F132" s="10"/>
-      <c r="G132" s="11"/>
+      <c r="B132" s="8"/>
+      <c r="C132" s="9"/>
+      <c r="D132" s="9"/>
+      <c r="E132" s="9"/>
+      <c r="F132" s="9"/>
+      <c r="G132" s="10"/>
       <c r="H132" s="3"/>
       <c r="I132" s="3"/>
       <c r="J132" s="3"/>
@@ -2822,12 +2832,12 @@
       <c r="O132" s="3"/>
     </row>
     <row r="133" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B133" s="9"/>
-      <c r="C133" s="10"/>
-      <c r="D133" s="10"/>
-      <c r="E133" s="10"/>
-      <c r="F133" s="10"/>
-      <c r="G133" s="11"/>
+      <c r="B133" s="8"/>
+      <c r="C133" s="9"/>
+      <c r="D133" s="9"/>
+      <c r="E133" s="9"/>
+      <c r="F133" s="9"/>
+      <c r="G133" s="10"/>
       <c r="H133" s="3"/>
       <c r="I133" s="3"/>
       <c r="J133" s="3"/>
@@ -2838,12 +2848,12 @@
       <c r="O133" s="3"/>
     </row>
     <row r="134" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B134" s="9"/>
-      <c r="C134" s="10"/>
-      <c r="D134" s="10"/>
-      <c r="E134" s="10"/>
-      <c r="F134" s="10"/>
-      <c r="G134" s="11"/>
+      <c r="B134" s="8"/>
+      <c r="C134" s="9"/>
+      <c r="D134" s="9"/>
+      <c r="E134" s="9"/>
+      <c r="F134" s="9"/>
+      <c r="G134" s="10"/>
       <c r="H134" s="3"/>
       <c r="I134" s="3"/>
       <c r="J134" s="3"/>
@@ -2854,12 +2864,12 @@
       <c r="O134" s="3"/>
     </row>
     <row r="135" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B135" s="9"/>
-      <c r="C135" s="10"/>
-      <c r="D135" s="10"/>
-      <c r="E135" s="10"/>
-      <c r="F135" s="10"/>
-      <c r="G135" s="11"/>
+      <c r="B135" s="8"/>
+      <c r="C135" s="9"/>
+      <c r="D135" s="9"/>
+      <c r="E135" s="9"/>
+      <c r="F135" s="9"/>
+      <c r="G135" s="10"/>
       <c r="H135" s="3"/>
       <c r="I135" s="3"/>
       <c r="J135" s="3"/>
@@ -2870,12 +2880,12 @@
       <c r="O135" s="3"/>
     </row>
     <row r="136" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B136" s="9"/>
-      <c r="C136" s="10"/>
-      <c r="D136" s="10"/>
-      <c r="E136" s="10"/>
-      <c r="F136" s="10"/>
-      <c r="G136" s="11"/>
+      <c r="B136" s="8"/>
+      <c r="C136" s="9"/>
+      <c r="D136" s="9"/>
+      <c r="E136" s="9"/>
+      <c r="F136" s="9"/>
+      <c r="G136" s="10"/>
       <c r="H136" s="3"/>
       <c r="I136" s="3"/>
       <c r="J136" s="3"/>
@@ -2886,12 +2896,12 @@
       <c r="O136" s="3"/>
     </row>
     <row r="137" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B137" s="9"/>
-      <c r="C137" s="10"/>
-      <c r="D137" s="10"/>
-      <c r="E137" s="10"/>
-      <c r="F137" s="10"/>
-      <c r="G137" s="11"/>
+      <c r="B137" s="8"/>
+      <c r="C137" s="9"/>
+      <c r="D137" s="9"/>
+      <c r="E137" s="9"/>
+      <c r="F137" s="9"/>
+      <c r="G137" s="10"/>
       <c r="H137" s="3"/>
       <c r="I137" s="3"/>
       <c r="J137" s="3"/>
@@ -2902,12 +2912,12 @@
       <c r="O137" s="3"/>
     </row>
     <row r="138" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B138" s="9"/>
-      <c r="C138" s="10"/>
-      <c r="D138" s="10"/>
-      <c r="E138" s="10"/>
-      <c r="F138" s="10"/>
-      <c r="G138" s="11"/>
+      <c r="B138" s="8"/>
+      <c r="C138" s="9"/>
+      <c r="D138" s="9"/>
+      <c r="E138" s="9"/>
+      <c r="F138" s="9"/>
+      <c r="G138" s="10"/>
       <c r="H138" s="3"/>
       <c r="I138" s="3"/>
       <c r="J138" s="3"/>
@@ -2918,12 +2928,12 @@
       <c r="O138" s="3"/>
     </row>
     <row r="139" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B139" s="9"/>
-      <c r="C139" s="10"/>
-      <c r="D139" s="10"/>
-      <c r="E139" s="10"/>
-      <c r="F139" s="10"/>
-      <c r="G139" s="11"/>
+      <c r="B139" s="8"/>
+      <c r="C139" s="9"/>
+      <c r="D139" s="9"/>
+      <c r="E139" s="9"/>
+      <c r="F139" s="9"/>
+      <c r="G139" s="10"/>
       <c r="H139" s="3"/>
       <c r="I139" s="3"/>
       <c r="J139" s="3"/>
@@ -2934,12 +2944,12 @@
       <c r="O139" s="3"/>
     </row>
     <row r="140" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B140" s="9"/>
-      <c r="C140" s="10"/>
-      <c r="D140" s="10"/>
-      <c r="E140" s="10"/>
-      <c r="F140" s="10"/>
-      <c r="G140" s="11"/>
+      <c r="B140" s="8"/>
+      <c r="C140" s="9"/>
+      <c r="D140" s="9"/>
+      <c r="E140" s="9"/>
+      <c r="F140" s="9"/>
+      <c r="G140" s="10"/>
       <c r="H140" s="3"/>
       <c r="I140" s="3"/>
       <c r="J140" s="3"/>
@@ -2950,12 +2960,12 @@
       <c r="O140" s="3"/>
     </row>
     <row r="141" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B141" s="9"/>
-      <c r="C141" s="10"/>
-      <c r="D141" s="10"/>
-      <c r="E141" s="10"/>
-      <c r="F141" s="10"/>
-      <c r="G141" s="11"/>
+      <c r="B141" s="8"/>
+      <c r="C141" s="9"/>
+      <c r="D141" s="9"/>
+      <c r="E141" s="9"/>
+      <c r="F141" s="9"/>
+      <c r="G141" s="10"/>
       <c r="H141" s="3"/>
       <c r="I141" s="3"/>
       <c r="J141" s="3"/>
@@ -2966,12 +2976,12 @@
       <c r="O141" s="3"/>
     </row>
     <row r="142" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B142" s="9"/>
-      <c r="C142" s="10"/>
-      <c r="D142" s="10"/>
-      <c r="E142" s="10"/>
-      <c r="F142" s="10"/>
-      <c r="G142" s="11"/>
+      <c r="B142" s="8"/>
+      <c r="C142" s="9"/>
+      <c r="D142" s="9"/>
+      <c r="E142" s="9"/>
+      <c r="F142" s="9"/>
+      <c r="G142" s="10"/>
       <c r="H142" s="3"/>
       <c r="I142" s="3"/>
       <c r="J142" s="3"/>
@@ -2982,12 +2992,12 @@
       <c r="O142" s="3"/>
     </row>
     <row r="143" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B143" s="9"/>
-      <c r="C143" s="10"/>
-      <c r="D143" s="10"/>
-      <c r="E143" s="10"/>
-      <c r="F143" s="10"/>
-      <c r="G143" s="11"/>
+      <c r="B143" s="8"/>
+      <c r="C143" s="9"/>
+      <c r="D143" s="9"/>
+      <c r="E143" s="9"/>
+      <c r="F143" s="9"/>
+      <c r="G143" s="10"/>
       <c r="H143" s="3"/>
       <c r="I143" s="3"/>
       <c r="J143" s="3"/>
@@ -2998,12 +3008,12 @@
       <c r="O143" s="3"/>
     </row>
     <row r="144" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B144" s="9"/>
-      <c r="C144" s="10"/>
-      <c r="D144" s="10"/>
-      <c r="E144" s="10"/>
-      <c r="F144" s="10"/>
-      <c r="G144" s="11"/>
+      <c r="B144" s="8"/>
+      <c r="C144" s="9"/>
+      <c r="D144" s="9"/>
+      <c r="E144" s="9"/>
+      <c r="F144" s="9"/>
+      <c r="G144" s="10"/>
       <c r="H144" s="3"/>
       <c r="I144" s="3"/>
       <c r="J144" s="3"/>
@@ -3014,12 +3024,12 @@
       <c r="O144" s="3"/>
     </row>
     <row r="145" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B145" s="9"/>
-      <c r="C145" s="10"/>
-      <c r="D145" s="10"/>
-      <c r="E145" s="10"/>
-      <c r="F145" s="10"/>
-      <c r="G145" s="11"/>
+      <c r="B145" s="8"/>
+      <c r="C145" s="9"/>
+      <c r="D145" s="9"/>
+      <c r="E145" s="9"/>
+      <c r="F145" s="9"/>
+      <c r="G145" s="10"/>
       <c r="H145" s="3"/>
       <c r="I145" s="3"/>
       <c r="J145" s="3"/>
@@ -3030,12 +3040,12 @@
       <c r="O145" s="3"/>
     </row>
     <row r="146" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B146" s="9"/>
-      <c r="C146" s="10"/>
-      <c r="D146" s="10"/>
-      <c r="E146" s="10"/>
-      <c r="F146" s="10"/>
-      <c r="G146" s="11"/>
+      <c r="B146" s="8"/>
+      <c r="C146" s="9"/>
+      <c r="D146" s="9"/>
+      <c r="E146" s="9"/>
+      <c r="F146" s="9"/>
+      <c r="G146" s="10"/>
       <c r="H146" s="3"/>
       <c r="I146" s="3"/>
       <c r="J146" s="3"/>
@@ -3046,12 +3056,12 @@
       <c r="O146" s="3"/>
     </row>
     <row r="147" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B147" s="9"/>
-      <c r="C147" s="10"/>
-      <c r="D147" s="10"/>
-      <c r="E147" s="10"/>
-      <c r="F147" s="10"/>
-      <c r="G147" s="11"/>
+      <c r="B147" s="8"/>
+      <c r="C147" s="9"/>
+      <c r="D147" s="9"/>
+      <c r="E147" s="9"/>
+      <c r="F147" s="9"/>
+      <c r="G147" s="10"/>
       <c r="H147" s="3"/>
       <c r="I147" s="3"/>
       <c r="J147" s="3"/>
@@ -3062,12 +3072,12 @@
       <c r="O147" s="3"/>
     </row>
     <row r="148" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B148" s="9"/>
-      <c r="C148" s="10"/>
-      <c r="D148" s="10"/>
-      <c r="E148" s="10"/>
-      <c r="F148" s="10"/>
-      <c r="G148" s="11"/>
+      <c r="B148" s="8"/>
+      <c r="C148" s="9"/>
+      <c r="D148" s="9"/>
+      <c r="E148" s="9"/>
+      <c r="F148" s="9"/>
+      <c r="G148" s="10"/>
       <c r="H148" s="3"/>
       <c r="I148" s="3"/>
       <c r="J148" s="3"/>
@@ -3078,12 +3088,12 @@
       <c r="O148" s="3"/>
     </row>
     <row r="149" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B149" s="9"/>
-      <c r="C149" s="10"/>
-      <c r="D149" s="10"/>
-      <c r="E149" s="10"/>
-      <c r="F149" s="10"/>
-      <c r="G149" s="11"/>
+      <c r="B149" s="8"/>
+      <c r="C149" s="9"/>
+      <c r="D149" s="9"/>
+      <c r="E149" s="9"/>
+      <c r="F149" s="9"/>
+      <c r="G149" s="10"/>
       <c r="H149" s="3"/>
       <c r="I149" s="3"/>
       <c r="J149" s="3"/>
@@ -3094,12 +3104,12 @@
       <c r="O149" s="3"/>
     </row>
     <row r="150" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B150" s="9"/>
-      <c r="C150" s="10"/>
-      <c r="D150" s="10"/>
-      <c r="E150" s="10"/>
-      <c r="F150" s="10"/>
-      <c r="G150" s="11"/>
+      <c r="B150" s="8"/>
+      <c r="C150" s="9"/>
+      <c r="D150" s="9"/>
+      <c r="E150" s="9"/>
+      <c r="F150" s="9"/>
+      <c r="G150" s="10"/>
       <c r="H150" s="3"/>
       <c r="I150" s="3"/>
       <c r="J150" s="3"/>
@@ -3110,12 +3120,12 @@
       <c r="O150" s="3"/>
     </row>
     <row r="151" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B151" s="9"/>
-      <c r="C151" s="10"/>
-      <c r="D151" s="10"/>
-      <c r="E151" s="10"/>
-      <c r="F151" s="10"/>
-      <c r="G151" s="11"/>
+      <c r="B151" s="8"/>
+      <c r="C151" s="9"/>
+      <c r="D151" s="9"/>
+      <c r="E151" s="9"/>
+      <c r="F151" s="9"/>
+      <c r="G151" s="10"/>
       <c r="H151" s="3"/>
       <c r="I151" s="3"/>
       <c r="J151" s="3"/>
@@ -3126,12 +3136,12 @@
       <c r="O151" s="3"/>
     </row>
     <row r="152" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B152" s="9"/>
-      <c r="C152" s="10"/>
-      <c r="D152" s="10"/>
-      <c r="E152" s="10"/>
-      <c r="F152" s="10"/>
-      <c r="G152" s="11"/>
+      <c r="B152" s="8"/>
+      <c r="C152" s="9"/>
+      <c r="D152" s="9"/>
+      <c r="E152" s="9"/>
+      <c r="F152" s="9"/>
+      <c r="G152" s="10"/>
       <c r="H152" s="3"/>
       <c r="I152" s="3"/>
       <c r="J152" s="3"/>
@@ -3142,12 +3152,12 @@
       <c r="O152" s="3"/>
     </row>
     <row r="153" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B153" s="9"/>
-      <c r="C153" s="10"/>
-      <c r="D153" s="10"/>
-      <c r="E153" s="10"/>
-      <c r="F153" s="10"/>
-      <c r="G153" s="11"/>
+      <c r="B153" s="8"/>
+      <c r="C153" s="9"/>
+      <c r="D153" s="9"/>
+      <c r="E153" s="9"/>
+      <c r="F153" s="9"/>
+      <c r="G153" s="10"/>
       <c r="H153" s="3"/>
       <c r="I153" s="3"/>
       <c r="J153" s="3"/>
@@ -3158,12 +3168,12 @@
       <c r="O153" s="3"/>
     </row>
     <row r="154" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B154" s="9"/>
-      <c r="C154" s="10"/>
-      <c r="D154" s="10"/>
-      <c r="E154" s="10"/>
-      <c r="F154" s="10"/>
-      <c r="G154" s="11"/>
+      <c r="B154" s="8"/>
+      <c r="C154" s="9"/>
+      <c r="D154" s="9"/>
+      <c r="E154" s="9"/>
+      <c r="F154" s="9"/>
+      <c r="G154" s="10"/>
       <c r="H154" s="3"/>
       <c r="I154" s="3"/>
       <c r="J154" s="3"/>
@@ -3174,12 +3184,12 @@
       <c r="O154" s="3"/>
     </row>
     <row r="155" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B155" s="9"/>
-      <c r="C155" s="10"/>
-      <c r="D155" s="10"/>
-      <c r="E155" s="10"/>
-      <c r="F155" s="10"/>
-      <c r="G155" s="11"/>
+      <c r="B155" s="8"/>
+      <c r="C155" s="9"/>
+      <c r="D155" s="9"/>
+      <c r="E155" s="9"/>
+      <c r="F155" s="9"/>
+      <c r="G155" s="10"/>
       <c r="H155" s="3"/>
       <c r="I155" s="3"/>
       <c r="J155" s="3"/>
@@ -3190,12 +3200,12 @@
       <c r="O155" s="3"/>
     </row>
     <row r="156" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B156" s="9"/>
-      <c r="C156" s="10"/>
-      <c r="D156" s="10"/>
-      <c r="E156" s="10"/>
-      <c r="F156" s="10"/>
-      <c r="G156" s="11"/>
+      <c r="B156" s="8"/>
+      <c r="C156" s="9"/>
+      <c r="D156" s="9"/>
+      <c r="E156" s="9"/>
+      <c r="F156" s="9"/>
+      <c r="G156" s="10"/>
       <c r="H156" s="3"/>
       <c r="I156" s="3"/>
       <c r="J156" s="3"/>
@@ -3206,12 +3216,12 @@
       <c r="O156" s="3"/>
     </row>
     <row r="157" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B157" s="9"/>
-      <c r="C157" s="10"/>
-      <c r="D157" s="10"/>
-      <c r="E157" s="10"/>
-      <c r="F157" s="10"/>
-      <c r="G157" s="11"/>
+      <c r="B157" s="8"/>
+      <c r="C157" s="9"/>
+      <c r="D157" s="9"/>
+      <c r="E157" s="9"/>
+      <c r="F157" s="9"/>
+      <c r="G157" s="10"/>
       <c r="H157" s="3"/>
       <c r="I157" s="3"/>
       <c r="J157" s="3"/>
@@ -3222,12 +3232,12 @@
       <c r="O157" s="3"/>
     </row>
     <row r="158" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B158" s="9"/>
-      <c r="C158" s="10"/>
-      <c r="D158" s="10"/>
-      <c r="E158" s="10"/>
-      <c r="F158" s="10"/>
-      <c r="G158" s="11"/>
+      <c r="B158" s="8"/>
+      <c r="C158" s="9"/>
+      <c r="D158" s="9"/>
+      <c r="E158" s="9"/>
+      <c r="F158" s="9"/>
+      <c r="G158" s="10"/>
       <c r="H158" s="3"/>
       <c r="I158" s="3"/>
       <c r="J158" s="3"/>
@@ -3238,12 +3248,12 @@
       <c r="O158" s="3"/>
     </row>
     <row r="159" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B159" s="9"/>
-      <c r="C159" s="10"/>
-      <c r="D159" s="10"/>
-      <c r="E159" s="10"/>
-      <c r="F159" s="10"/>
-      <c r="G159" s="11"/>
+      <c r="B159" s="8"/>
+      <c r="C159" s="9"/>
+      <c r="D159" s="9"/>
+      <c r="E159" s="9"/>
+      <c r="F159" s="9"/>
+      <c r="G159" s="10"/>
       <c r="H159" s="3"/>
       <c r="I159" s="3"/>
       <c r="J159" s="3"/>
@@ -3254,12 +3264,12 @@
       <c r="O159" s="3"/>
     </row>
     <row r="160" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B160" s="9"/>
-      <c r="C160" s="10"/>
-      <c r="D160" s="10"/>
-      <c r="E160" s="10"/>
-      <c r="F160" s="10"/>
-      <c r="G160" s="11"/>
+      <c r="B160" s="8"/>
+      <c r="C160" s="9"/>
+      <c r="D160" s="9"/>
+      <c r="E160" s="9"/>
+      <c r="F160" s="9"/>
+      <c r="G160" s="10"/>
       <c r="H160" s="3"/>
       <c r="I160" s="3"/>
       <c r="J160" s="3"/>
@@ -3270,12 +3280,12 @@
       <c r="O160" s="3"/>
     </row>
     <row r="161" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B161" s="9"/>
-      <c r="C161" s="10"/>
-      <c r="D161" s="10"/>
-      <c r="E161" s="10"/>
-      <c r="F161" s="10"/>
-      <c r="G161" s="11"/>
+      <c r="B161" s="8"/>
+      <c r="C161" s="9"/>
+      <c r="D161" s="9"/>
+      <c r="E161" s="9"/>
+      <c r="F161" s="9"/>
+      <c r="G161" s="10"/>
       <c r="H161" s="3"/>
       <c r="I161" s="3"/>
       <c r="J161" s="3"/>
@@ -3286,12 +3296,12 @@
       <c r="O161" s="3"/>
     </row>
     <row r="162" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B162" s="9"/>
-      <c r="C162" s="10"/>
-      <c r="D162" s="10"/>
-      <c r="E162" s="10"/>
-      <c r="F162" s="10"/>
-      <c r="G162" s="11"/>
+      <c r="B162" s="8"/>
+      <c r="C162" s="9"/>
+      <c r="D162" s="9"/>
+      <c r="E162" s="9"/>
+      <c r="F162" s="9"/>
+      <c r="G162" s="10"/>
       <c r="H162" s="3"/>
       <c r="I162" s="3"/>
       <c r="J162" s="3"/>
@@ -3302,12 +3312,12 @@
       <c r="O162" s="3"/>
     </row>
     <row r="163" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B163" s="9"/>
-      <c r="C163" s="10"/>
-      <c r="D163" s="10"/>
-      <c r="E163" s="10"/>
-      <c r="F163" s="10"/>
-      <c r="G163" s="11"/>
+      <c r="B163" s="8"/>
+      <c r="C163" s="9"/>
+      <c r="D163" s="9"/>
+      <c r="E163" s="9"/>
+      <c r="F163" s="9"/>
+      <c r="G163" s="10"/>
       <c r="H163" s="3"/>
       <c r="I163" s="3"/>
       <c r="J163" s="3"/>
@@ -3318,12 +3328,12 @@
       <c r="O163" s="3"/>
     </row>
     <row r="164" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B164" s="9"/>
-      <c r="C164" s="10"/>
-      <c r="D164" s="10"/>
-      <c r="E164" s="10"/>
-      <c r="F164" s="10"/>
-      <c r="G164" s="11"/>
+      <c r="B164" s="8"/>
+      <c r="C164" s="9"/>
+      <c r="D164" s="9"/>
+      <c r="E164" s="9"/>
+      <c r="F164" s="9"/>
+      <c r="G164" s="10"/>
       <c r="H164" s="3"/>
       <c r="I164" s="3"/>
       <c r="J164" s="3"/>
@@ -3334,12 +3344,12 @@
       <c r="O164" s="3"/>
     </row>
     <row r="165" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B165" s="9"/>
-      <c r="C165" s="10"/>
-      <c r="D165" s="10"/>
-      <c r="E165" s="10"/>
-      <c r="F165" s="10"/>
-      <c r="G165" s="11"/>
+      <c r="B165" s="8"/>
+      <c r="C165" s="9"/>
+      <c r="D165" s="9"/>
+      <c r="E165" s="9"/>
+      <c r="F165" s="9"/>
+      <c r="G165" s="10"/>
       <c r="H165" s="3"/>
       <c r="I165" s="3"/>
       <c r="J165" s="3"/>
@@ -3350,12 +3360,12 @@
       <c r="O165" s="3"/>
     </row>
     <row r="166" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B166" s="9"/>
-      <c r="C166" s="10"/>
-      <c r="D166" s="10"/>
-      <c r="E166" s="10"/>
-      <c r="F166" s="10"/>
-      <c r="G166" s="11"/>
+      <c r="B166" s="8"/>
+      <c r="C166" s="9"/>
+      <c r="D166" s="9"/>
+      <c r="E166" s="9"/>
+      <c r="F166" s="9"/>
+      <c r="G166" s="10"/>
       <c r="H166" s="3"/>
       <c r="I166" s="3"/>
       <c r="J166" s="3"/>
@@ -3366,12 +3376,12 @@
       <c r="O166" s="3"/>
     </row>
     <row r="167" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B167" s="9"/>
-      <c r="C167" s="10"/>
-      <c r="D167" s="10"/>
-      <c r="E167" s="10"/>
-      <c r="F167" s="10"/>
-      <c r="G167" s="11"/>
+      <c r="B167" s="8"/>
+      <c r="C167" s="9"/>
+      <c r="D167" s="9"/>
+      <c r="E167" s="9"/>
+      <c r="F167" s="9"/>
+      <c r="G167" s="10"/>
       <c r="H167" s="3"/>
       <c r="I167" s="3"/>
       <c r="J167" s="3"/>
@@ -3382,12 +3392,12 @@
       <c r="O167" s="3"/>
     </row>
     <row r="168" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B168" s="9"/>
-      <c r="C168" s="10"/>
-      <c r="D168" s="10"/>
-      <c r="E168" s="10"/>
-      <c r="F168" s="10"/>
-      <c r="G168" s="11"/>
+      <c r="B168" s="8"/>
+      <c r="C168" s="9"/>
+      <c r="D168" s="9"/>
+      <c r="E168" s="9"/>
+      <c r="F168" s="9"/>
+      <c r="G168" s="10"/>
       <c r="H168" s="3"/>
       <c r="I168" s="3"/>
       <c r="J168" s="3"/>
@@ -3398,12 +3408,12 @@
       <c r="O168" s="3"/>
     </row>
     <row r="169" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B169" s="9"/>
-      <c r="C169" s="10"/>
-      <c r="D169" s="10"/>
-      <c r="E169" s="10"/>
-      <c r="F169" s="10"/>
-      <c r="G169" s="11"/>
+      <c r="B169" s="8"/>
+      <c r="C169" s="9"/>
+      <c r="D169" s="9"/>
+      <c r="E169" s="9"/>
+      <c r="F169" s="9"/>
+      <c r="G169" s="10"/>
       <c r="H169" s="3"/>
       <c r="I169" s="3"/>
       <c r="J169" s="3"/>
@@ -3414,12 +3424,12 @@
       <c r="O169" s="3"/>
     </row>
     <row r="170" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B170" s="9"/>
-      <c r="C170" s="10"/>
-      <c r="D170" s="10"/>
-      <c r="E170" s="10"/>
-      <c r="F170" s="10"/>
-      <c r="G170" s="11"/>
+      <c r="B170" s="8"/>
+      <c r="C170" s="9"/>
+      <c r="D170" s="9"/>
+      <c r="E170" s="9"/>
+      <c r="F170" s="9"/>
+      <c r="G170" s="10"/>
       <c r="H170" s="3"/>
       <c r="I170" s="3"/>
       <c r="J170" s="3"/>
@@ -3430,12 +3440,12 @@
       <c r="O170" s="3"/>
     </row>
     <row r="171" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B171" s="9"/>
-      <c r="C171" s="10"/>
-      <c r="D171" s="10"/>
-      <c r="E171" s="10"/>
-      <c r="F171" s="10"/>
-      <c r="G171" s="11"/>
+      <c r="B171" s="8"/>
+      <c r="C171" s="9"/>
+      <c r="D171" s="9"/>
+      <c r="E171" s="9"/>
+      <c r="F171" s="9"/>
+      <c r="G171" s="10"/>
       <c r="H171" s="3"/>
       <c r="I171" s="3"/>
       <c r="J171" s="3"/>
@@ -3446,12 +3456,12 @@
       <c r="O171" s="3"/>
     </row>
     <row r="172" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B172" s="9"/>
-      <c r="C172" s="10"/>
-      <c r="D172" s="10"/>
-      <c r="E172" s="10"/>
-      <c r="F172" s="10"/>
-      <c r="G172" s="11"/>
+      <c r="B172" s="8"/>
+      <c r="C172" s="9"/>
+      <c r="D172" s="9"/>
+      <c r="E172" s="9"/>
+      <c r="F172" s="9"/>
+      <c r="G172" s="10"/>
       <c r="H172" s="3"/>
       <c r="I172" s="3"/>
       <c r="J172" s="3"/>
@@ -3462,12 +3472,12 @@
       <c r="O172" s="3"/>
     </row>
     <row r="173" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B173" s="9"/>
-      <c r="C173" s="10"/>
-      <c r="D173" s="10"/>
-      <c r="E173" s="10"/>
-      <c r="F173" s="10"/>
-      <c r="G173" s="11"/>
+      <c r="B173" s="8"/>
+      <c r="C173" s="9"/>
+      <c r="D173" s="9"/>
+      <c r="E173" s="9"/>
+      <c r="F173" s="9"/>
+      <c r="G173" s="10"/>
       <c r="H173" s="3"/>
       <c r="I173" s="3"/>
       <c r="J173" s="3"/>
@@ -3478,12 +3488,12 @@
       <c r="O173" s="3"/>
     </row>
     <row r="174" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B174" s="9"/>
-      <c r="C174" s="10"/>
-      <c r="D174" s="10"/>
-      <c r="E174" s="10"/>
-      <c r="F174" s="10"/>
-      <c r="G174" s="11"/>
+      <c r="B174" s="8"/>
+      <c r="C174" s="9"/>
+      <c r="D174" s="9"/>
+      <c r="E174" s="9"/>
+      <c r="F174" s="9"/>
+      <c r="G174" s="10"/>
       <c r="H174" s="3"/>
       <c r="I174" s="3"/>
       <c r="J174" s="3"/>
@@ -3494,12 +3504,12 @@
       <c r="O174" s="3"/>
     </row>
     <row r="175" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B175" s="9"/>
-      <c r="C175" s="10"/>
-      <c r="D175" s="10"/>
-      <c r="E175" s="10"/>
-      <c r="F175" s="10"/>
-      <c r="G175" s="11"/>
+      <c r="B175" s="8"/>
+      <c r="C175" s="9"/>
+      <c r="D175" s="9"/>
+      <c r="E175" s="9"/>
+      <c r="F175" s="9"/>
+      <c r="G175" s="10"/>
       <c r="H175" s="3"/>
       <c r="I175" s="3"/>
       <c r="J175" s="3"/>
@@ -3510,12 +3520,12 @@
       <c r="O175" s="3"/>
     </row>
     <row r="176" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B176" s="9"/>
-      <c r="C176" s="10"/>
-      <c r="D176" s="10"/>
-      <c r="E176" s="10"/>
-      <c r="F176" s="10"/>
-      <c r="G176" s="11"/>
+      <c r="B176" s="8"/>
+      <c r="C176" s="9"/>
+      <c r="D176" s="9"/>
+      <c r="E176" s="9"/>
+      <c r="F176" s="9"/>
+      <c r="G176" s="10"/>
       <c r="H176" s="3"/>
       <c r="I176" s="3"/>
       <c r="J176" s="3"/>
@@ -3526,12 +3536,12 @@
       <c r="O176" s="3"/>
     </row>
     <row r="177" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B177" s="9"/>
-      <c r="C177" s="10"/>
-      <c r="D177" s="10"/>
-      <c r="E177" s="10"/>
-      <c r="F177" s="10"/>
-      <c r="G177" s="11"/>
+      <c r="B177" s="8"/>
+      <c r="C177" s="9"/>
+      <c r="D177" s="9"/>
+      <c r="E177" s="9"/>
+      <c r="F177" s="9"/>
+      <c r="G177" s="10"/>
       <c r="H177" s="3"/>
       <c r="I177" s="3"/>
       <c r="J177" s="3"/>
@@ -3542,12 +3552,12 @@
       <c r="O177" s="3"/>
     </row>
     <row r="178" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B178" s="9"/>
-      <c r="C178" s="10"/>
-      <c r="D178" s="10"/>
-      <c r="E178" s="10"/>
-      <c r="F178" s="10"/>
-      <c r="G178" s="11"/>
+      <c r="B178" s="8"/>
+      <c r="C178" s="9"/>
+      <c r="D178" s="9"/>
+      <c r="E178" s="9"/>
+      <c r="F178" s="9"/>
+      <c r="G178" s="10"/>
       <c r="H178" s="3"/>
       <c r="I178" s="3"/>
       <c r="J178" s="3"/>
@@ -3558,12 +3568,12 @@
       <c r="O178" s="3"/>
     </row>
     <row r="179" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B179" s="9"/>
-      <c r="C179" s="10"/>
-      <c r="D179" s="10"/>
-      <c r="E179" s="10"/>
-      <c r="F179" s="10"/>
-      <c r="G179" s="11"/>
+      <c r="B179" s="8"/>
+      <c r="C179" s="9"/>
+      <c r="D179" s="9"/>
+      <c r="E179" s="9"/>
+      <c r="F179" s="9"/>
+      <c r="G179" s="10"/>
       <c r="H179" s="3"/>
       <c r="I179" s="3"/>
       <c r="J179" s="3"/>
@@ -3574,12 +3584,12 @@
       <c r="O179" s="3"/>
     </row>
     <row r="180" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B180" s="9"/>
-      <c r="C180" s="10"/>
-      <c r="D180" s="10"/>
-      <c r="E180" s="10"/>
-      <c r="F180" s="10"/>
-      <c r="G180" s="11"/>
+      <c r="B180" s="8"/>
+      <c r="C180" s="9"/>
+      <c r="D180" s="9"/>
+      <c r="E180" s="9"/>
+      <c r="F180" s="9"/>
+      <c r="G180" s="10"/>
       <c r="H180" s="3"/>
       <c r="I180" s="3"/>
       <c r="J180" s="3"/>
@@ -3590,12 +3600,12 @@
       <c r="O180" s="3"/>
     </row>
     <row r="181" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B181" s="9"/>
-      <c r="C181" s="10"/>
-      <c r="D181" s="10"/>
-      <c r="E181" s="10"/>
-      <c r="F181" s="10"/>
-      <c r="G181" s="11"/>
+      <c r="B181" s="8"/>
+      <c r="C181" s="9"/>
+      <c r="D181" s="9"/>
+      <c r="E181" s="9"/>
+      <c r="F181" s="9"/>
+      <c r="G181" s="10"/>
       <c r="H181" s="3"/>
       <c r="I181" s="3"/>
       <c r="J181" s="3"/>
@@ -3606,12 +3616,12 @@
       <c r="O181" s="3"/>
     </row>
     <row r="182" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B182" s="9"/>
-      <c r="C182" s="10"/>
-      <c r="D182" s="10"/>
-      <c r="E182" s="10"/>
-      <c r="F182" s="10"/>
-      <c r="G182" s="11"/>
+      <c r="B182" s="8"/>
+      <c r="C182" s="9"/>
+      <c r="D182" s="9"/>
+      <c r="E182" s="9"/>
+      <c r="F182" s="9"/>
+      <c r="G182" s="10"/>
       <c r="H182" s="3"/>
       <c r="I182" s="3"/>
       <c r="J182" s="3"/>
@@ -3622,12 +3632,12 @@
       <c r="O182" s="3"/>
     </row>
     <row r="183" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B183" s="9"/>
-      <c r="C183" s="10"/>
-      <c r="D183" s="10"/>
-      <c r="E183" s="10"/>
-      <c r="F183" s="10"/>
-      <c r="G183" s="11"/>
+      <c r="B183" s="8"/>
+      <c r="C183" s="9"/>
+      <c r="D183" s="9"/>
+      <c r="E183" s="9"/>
+      <c r="F183" s="9"/>
+      <c r="G183" s="10"/>
       <c r="H183" s="3"/>
       <c r="I183" s="3"/>
       <c r="J183" s="3"/>
@@ -3638,12 +3648,12 @@
       <c r="O183" s="3"/>
     </row>
     <row r="184" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B184" s="9"/>
-      <c r="C184" s="10"/>
-      <c r="D184" s="10"/>
-      <c r="E184" s="10"/>
-      <c r="F184" s="10"/>
-      <c r="G184" s="11"/>
+      <c r="B184" s="8"/>
+      <c r="C184" s="9"/>
+      <c r="D184" s="9"/>
+      <c r="E184" s="9"/>
+      <c r="F184" s="9"/>
+      <c r="G184" s="10"/>
       <c r="H184" s="3"/>
       <c r="I184" s="3"/>
       <c r="J184" s="3"/>
@@ -3654,12 +3664,12 @@
       <c r="O184" s="3"/>
     </row>
     <row r="185" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B185" s="9"/>
-      <c r="C185" s="10"/>
-      <c r="D185" s="10"/>
-      <c r="E185" s="10"/>
-      <c r="F185" s="10"/>
-      <c r="G185" s="11"/>
+      <c r="B185" s="8"/>
+      <c r="C185" s="9"/>
+      <c r="D185" s="9"/>
+      <c r="E185" s="9"/>
+      <c r="F185" s="9"/>
+      <c r="G185" s="10"/>
       <c r="H185" s="3"/>
       <c r="I185" s="3"/>
       <c r="J185" s="3"/>
@@ -3670,12 +3680,12 @@
       <c r="O185" s="3"/>
     </row>
     <row r="186" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B186" s="9"/>
-      <c r="C186" s="10"/>
-      <c r="D186" s="10"/>
-      <c r="E186" s="10"/>
-      <c r="F186" s="10"/>
-      <c r="G186" s="11"/>
+      <c r="B186" s="8"/>
+      <c r="C186" s="9"/>
+      <c r="D186" s="9"/>
+      <c r="E186" s="9"/>
+      <c r="F186" s="9"/>
+      <c r="G186" s="10"/>
       <c r="H186" s="3"/>
       <c r="I186" s="3"/>
       <c r="J186" s="3"/>
@@ -3686,12 +3696,12 @@
       <c r="O186" s="3"/>
     </row>
     <row r="187" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B187" s="9"/>
-      <c r="C187" s="10"/>
-      <c r="D187" s="10"/>
-      <c r="E187" s="10"/>
-      <c r="F187" s="10"/>
-      <c r="G187" s="11"/>
+      <c r="B187" s="8"/>
+      <c r="C187" s="9"/>
+      <c r="D187" s="9"/>
+      <c r="E187" s="9"/>
+      <c r="F187" s="9"/>
+      <c r="G187" s="10"/>
       <c r="H187" s="3"/>
       <c r="I187" s="3"/>
       <c r="J187" s="3"/>
@@ -3702,12 +3712,12 @@
       <c r="O187" s="3"/>
     </row>
     <row r="188" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B188" s="9"/>
-      <c r="C188" s="10"/>
-      <c r="D188" s="10"/>
-      <c r="E188" s="10"/>
-      <c r="F188" s="10"/>
-      <c r="G188" s="11"/>
+      <c r="B188" s="8"/>
+      <c r="C188" s="9"/>
+      <c r="D188" s="9"/>
+      <c r="E188" s="9"/>
+      <c r="F188" s="9"/>
+      <c r="G188" s="10"/>
       <c r="H188" s="3"/>
       <c r="I188" s="3"/>
       <c r="J188" s="3"/>
@@ -3718,12 +3728,12 @@
       <c r="O188" s="3"/>
     </row>
     <row r="189" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B189" s="9"/>
-      <c r="C189" s="10"/>
-      <c r="D189" s="10"/>
-      <c r="E189" s="10"/>
-      <c r="F189" s="10"/>
-      <c r="G189" s="11"/>
+      <c r="B189" s="8"/>
+      <c r="C189" s="9"/>
+      <c r="D189" s="9"/>
+      <c r="E189" s="9"/>
+      <c r="F189" s="9"/>
+      <c r="G189" s="10"/>
       <c r="H189" s="3"/>
       <c r="I189" s="3"/>
       <c r="J189" s="3"/>
@@ -3734,12 +3744,12 @@
       <c r="O189" s="3"/>
     </row>
     <row r="190" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B190" s="9"/>
-      <c r="C190" s="10"/>
-      <c r="D190" s="10"/>
-      <c r="E190" s="10"/>
-      <c r="F190" s="10"/>
-      <c r="G190" s="11"/>
+      <c r="B190" s="8"/>
+      <c r="C190" s="9"/>
+      <c r="D190" s="9"/>
+      <c r="E190" s="9"/>
+      <c r="F190" s="9"/>
+      <c r="G190" s="10"/>
       <c r="H190" s="3"/>
       <c r="I190" s="3"/>
       <c r="J190" s="3"/>
@@ -3750,12 +3760,12 @@
       <c r="O190" s="3"/>
     </row>
     <row r="191" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B191" s="9"/>
-      <c r="C191" s="10"/>
-      <c r="D191" s="10"/>
-      <c r="E191" s="10"/>
-      <c r="F191" s="10"/>
-      <c r="G191" s="11"/>
+      <c r="B191" s="8"/>
+      <c r="C191" s="9"/>
+      <c r="D191" s="9"/>
+      <c r="E191" s="9"/>
+      <c r="F191" s="9"/>
+      <c r="G191" s="10"/>
       <c r="H191" s="3"/>
       <c r="I191" s="3"/>
       <c r="J191" s="3"/>
@@ -3766,12 +3776,12 @@
       <c r="O191" s="3"/>
     </row>
     <row r="192" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B192" s="9"/>
-      <c r="C192" s="10"/>
-      <c r="D192" s="10"/>
-      <c r="E192" s="10"/>
-      <c r="F192" s="10"/>
-      <c r="G192" s="11"/>
+      <c r="B192" s="8"/>
+      <c r="C192" s="9"/>
+      <c r="D192" s="9"/>
+      <c r="E192" s="9"/>
+      <c r="F192" s="9"/>
+      <c r="G192" s="10"/>
       <c r="H192" s="3"/>
       <c r="I192" s="3"/>
       <c r="J192" s="3"/>
@@ -3782,12 +3792,12 @@
       <c r="O192" s="3"/>
     </row>
     <row r="193" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B193" s="9"/>
-      <c r="C193" s="10"/>
-      <c r="D193" s="10"/>
-      <c r="E193" s="10"/>
-      <c r="F193" s="10"/>
-      <c r="G193" s="11"/>
+      <c r="B193" s="8"/>
+      <c r="C193" s="9"/>
+      <c r="D193" s="9"/>
+      <c r="E193" s="9"/>
+      <c r="F193" s="9"/>
+      <c r="G193" s="10"/>
       <c r="H193" s="3"/>
       <c r="I193" s="3"/>
       <c r="J193" s="3"/>
@@ -3798,12 +3808,12 @@
       <c r="O193" s="3"/>
     </row>
     <row r="194" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B194" s="9"/>
-      <c r="C194" s="10"/>
-      <c r="D194" s="10"/>
-      <c r="E194" s="10"/>
-      <c r="F194" s="10"/>
-      <c r="G194" s="11"/>
+      <c r="B194" s="8"/>
+      <c r="C194" s="9"/>
+      <c r="D194" s="9"/>
+      <c r="E194" s="9"/>
+      <c r="F194" s="9"/>
+      <c r="G194" s="10"/>
       <c r="H194" s="3"/>
       <c r="I194" s="3"/>
       <c r="J194" s="3"/>
@@ -3814,12 +3824,12 @@
       <c r="O194" s="3"/>
     </row>
     <row r="195" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B195" s="9"/>
-      <c r="C195" s="10"/>
-      <c r="D195" s="10"/>
-      <c r="E195" s="10"/>
-      <c r="F195" s="10"/>
-      <c r="G195" s="11"/>
+      <c r="B195" s="8"/>
+      <c r="C195" s="9"/>
+      <c r="D195" s="9"/>
+      <c r="E195" s="9"/>
+      <c r="F195" s="9"/>
+      <c r="G195" s="10"/>
       <c r="H195" s="3"/>
       <c r="I195" s="3"/>
       <c r="J195" s="3"/>
@@ -3830,12 +3840,12 @@
       <c r="O195" s="3"/>
     </row>
     <row r="196" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B196" s="9"/>
-      <c r="C196" s="10"/>
-      <c r="D196" s="10"/>
-      <c r="E196" s="10"/>
-      <c r="F196" s="10"/>
-      <c r="G196" s="11"/>
+      <c r="B196" s="8"/>
+      <c r="C196" s="9"/>
+      <c r="D196" s="9"/>
+      <c r="E196" s="9"/>
+      <c r="F196" s="9"/>
+      <c r="G196" s="10"/>
       <c r="H196" s="3"/>
       <c r="I196" s="3"/>
       <c r="J196" s="3"/>
@@ -3846,12 +3856,12 @@
       <c r="O196" s="3"/>
     </row>
     <row r="197" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B197" s="9"/>
-      <c r="C197" s="10"/>
-      <c r="D197" s="10"/>
-      <c r="E197" s="10"/>
-      <c r="F197" s="10"/>
-      <c r="G197" s="11"/>
+      <c r="B197" s="8"/>
+      <c r="C197" s="9"/>
+      <c r="D197" s="9"/>
+      <c r="E197" s="9"/>
+      <c r="F197" s="9"/>
+      <c r="G197" s="10"/>
       <c r="H197" s="3"/>
       <c r="I197" s="3"/>
       <c r="J197" s="3"/>
@@ -3862,12 +3872,12 @@
       <c r="O197" s="3"/>
     </row>
     <row r="198" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B198" s="9"/>
-      <c r="C198" s="10"/>
-      <c r="D198" s="10"/>
-      <c r="E198" s="10"/>
-      <c r="F198" s="10"/>
-      <c r="G198" s="11"/>
+      <c r="B198" s="8"/>
+      <c r="C198" s="9"/>
+      <c r="D198" s="9"/>
+      <c r="E198" s="9"/>
+      <c r="F198" s="9"/>
+      <c r="G198" s="10"/>
       <c r="H198" s="3"/>
       <c r="I198" s="3"/>
       <c r="J198" s="3"/>
@@ -3878,12 +3888,12 @@
       <c r="O198" s="3"/>
     </row>
     <row r="199" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B199" s="12"/>
-      <c r="C199" s="13"/>
-      <c r="D199" s="13"/>
-      <c r="E199" s="13"/>
-      <c r="F199" s="13"/>
-      <c r="G199" s="14"/>
+      <c r="B199" s="11"/>
+      <c r="C199" s="12"/>
+      <c r="D199" s="12"/>
+      <c r="E199" s="12"/>
+      <c r="F199" s="12"/>
+      <c r="G199" s="13"/>
       <c r="H199" s="3"/>
       <c r="I199" s="3"/>
       <c r="J199" s="3"/>

</xml_diff>